<commit_message>
Weitere Literatur hinzugefügt, Referenzdateien in ihre BibTex-Keys umbenannt, Grundlagenkapitel für die Algorithmen angefangen (Gerüst erstellt), Titelseite um Thema ergänzt, Fehlerhafte Messungen wiederholt und Tabellen angepasst
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
   <si>
     <t>Unoptimized</t>
   </si>
@@ -96,10 +96,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -211,28 +211,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1532</c:v>
+                  <c:v>2191</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>822</c:v>
+                  <c:v>873</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3346</c:v>
+                  <c:v>4650</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2001</c:v>
+                  <c:v>2096</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>176</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>63</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2113</c:v>
+                  <c:v>2070</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>827</c:v>
+                  <c:v>736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -307,7 +307,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5.64</c:v>
+                  <c:v>5.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
@@ -430,28 +430,27 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="58739328"/>
-        <c:axId val="58757504"/>
+        <c:axId val="58107392"/>
+        <c:axId val="58108928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58739328"/>
+        <c:axId val="58107392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58757504"/>
+        <c:crossAx val="58108928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58757504"/>
+        <c:axId val="58108928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4000"/>
@@ -480,7 +479,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58739328"/>
+        <c:crossAx val="58107392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -495,7 +494,412 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Laufzeitmessungen auf dem ARM ohne aktive Optimierung </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Extraction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Tabelle1!$K$1:$R$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>FeatureSet 1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>FeatureSet 2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>FeatureSet 3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>FeatureSet 4</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$K$3:$R$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>99.337368519103805</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.537702669822366</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.42061163940788</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.729469075526183</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84.567600631881504</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84.644664344228687</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>94.675591114142364</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94.289900962295064</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Processing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Tabelle1!$K$1:$R$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>FeatureSet 1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>FeatureSet 2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>FeatureSet 3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>FeatureSet 4</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$K$4:$R$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.24029577962174814</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17102698053234086</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.40226571257087</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.161348654468938</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.008041048543229</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.982510296229872</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.8984327576447564</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.3832359217875529</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$J$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Classification</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Tabelle1!$K$1:$R$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>FeatureSet 1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>FeatureSet 2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>FeatureSet 3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>FeatureSet 4</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$K$5:$R$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.42233570127444264</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29127034964527865</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17712264802123798</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10918227000487689</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4243583195752612</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3728253595414373</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.42597612821288705</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.32686311591739081</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:gapWidth val="75"/>
+        <c:overlap val="100"/>
+        <c:axId val="64968960"/>
+        <c:axId val="64978944"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="64968960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64978944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="64978944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Anteil in [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64968960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -528,6 +932,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>752474</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -821,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -840,27 +1274,44 @@
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="3"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" s="3"/>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -885,42 +1336,102 @@
       <c r="I2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1532</v>
+        <v>2191</v>
       </c>
       <c r="C3" s="1">
-        <v>822</v>
+        <v>873</v>
       </c>
       <c r="D3" s="1">
-        <v>3346</v>
+        <v>4650</v>
       </c>
       <c r="E3" s="1">
-        <v>2001</v>
+        <v>2096</v>
       </c>
       <c r="F3" s="1">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G3" s="1">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H3" s="1">
-        <v>2113</v>
+        <v>2070</v>
       </c>
       <c r="I3" s="1">
-        <v>827</v>
+        <v>736</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
+        <f>B3/K6*100</f>
+        <v>99.337368519103805</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:R3" si="0">C3/L6*100</f>
+        <v>99.537702669822366</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" si="0"/>
+        <v>88.42061163940788</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" si="0"/>
+        <v>89.729469075526183</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" si="0"/>
+        <v>84.567600631881504</v>
+      </c>
+      <c r="P3" s="1">
+        <f t="shared" si="0"/>
+        <v>84.644664344228687</v>
+      </c>
+      <c r="Q3" s="1">
+        <f t="shared" si="0"/>
+        <v>94.675591114142364</v>
+      </c>
+      <c r="R3" s="1">
+        <f t="shared" si="0"/>
+        <v>94.289900962295064</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>5.64</v>
+        <v>5.3</v>
       </c>
       <c r="C4" s="1">
         <v>1.5</v>
@@ -943,8 +1454,43 @@
       <c r="I4" s="1">
         <v>42.02</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1">
+        <f>B4/K6*100</f>
+        <v>0.24029577962174814</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" ref="L4:R4" si="1">C4/L6*100</f>
+        <v>0.17102698053234086</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" si="1"/>
+        <v>11.40226571257087</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" si="1"/>
+        <v>10.161348654468938</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="1"/>
+        <v>11.008041048543229</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" si="1"/>
+        <v>11.982510296229872</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8984327576447564</v>
+      </c>
+      <c r="R4" s="1">
+        <f t="shared" si="1"/>
+        <v>5.3832359217875529</v>
+      </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -972,13 +1518,86 @@
       <c r="I5" s="1">
         <v>2.5514000000000001</v>
       </c>
+      <c r="J5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1">
+        <f>B5/K6*100</f>
+        <v>0.42233570127444264</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" ref="L5:R5" si="2">C5/L6*100</f>
+        <v>0.29127034964527865</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.17712264802123798</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10918227000487689</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="2"/>
+        <v>4.4243583195752612</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="2"/>
+        <v>3.3728253595414373</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.42597612821288705</v>
+      </c>
+      <c r="R5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.32686311591739081</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="K6">
+        <f>SUM(B3:B5)</f>
+        <v>2205.6151</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ref="L6:R6" si="3">SUM(C3:C5)</f>
+        <v>877.05460000000005</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>5258.9548000000004</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>2335.9104000000002</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="3"/>
+        <v>210.48250000000002</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="3"/>
+        <v>75.610200000000006</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="3"/>
+        <v>2186.4135999999999</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="3"/>
+        <v>780.57139999999993</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Kapitel Ergebnisse und Zusammenfassung hinzugefügt, Optimisierung und Grundlagen weitergeschrieben, Bilder aus den Result-Tabellen hinzu- ung eingefügt
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -432,25 +432,25 @@
         </c:ser>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="58107392"/>
-        <c:axId val="58108928"/>
+        <c:axId val="52521216"/>
+        <c:axId val="52573696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58107392"/>
+        <c:axId val="52521216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58108928"/>
+        <c:crossAx val="52573696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58108928"/>
+        <c:axId val="52573696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4000"/>
@@ -479,7 +479,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58107392"/>
+        <c:crossAx val="52521216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -494,7 +494,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -505,45 +505,7 @@
   <c:lang val="de-DE"/>
   <c:style val="18"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="1" i="0" baseline="0"/>
-              <a:t>Laufzeitmessungen auf dem ARM ohne aktive Optimierung </a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -837,31 +799,31 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="64968960"/>
-        <c:axId val="64978944"/>
+        <c:axId val="54568064"/>
+        <c:axId val="54570368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="64968960"/>
+        <c:axId val="54568064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64978944"/>
+        <c:crossAx val="54570368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64978944"/>
+        <c:axId val="54570368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
+          <c:min val="80"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -886,7 +848,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64968960"/>
+        <c:crossAx val="54568064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -899,8 +861,8 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1600,8 +1562,8 @@
     <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1614,7 +1576,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1627,6 +1589,6 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Libav gemessen und die Result-Tabellen auf den neusten Stand gebracht
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="10">
   <si>
     <t>Unoptimized</t>
   </si>
@@ -44,6 +44,9 @@
   <si>
     <t>FeatureSet 4</t>
   </si>
+  <si>
+    <t>NEON FFT Optimized</t>
+  </si>
 </sst>
 </file>
 
@@ -66,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -89,17 +92,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -158,9 +208,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$B$1:$I$2</c:f>
+              <c:f>Tabelle1!$B$1:$M$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -169,35 +219,47 @@
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>NEON FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="9">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -206,10 +268,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$3:$I$3</c:f>
+              <c:f>Tabelle1!$B$3:$M$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2191</c:v>
                 </c:pt>
@@ -217,22 +279,34 @@
                   <c:v>873</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4650</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2096</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>659</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>178</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2070</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>106</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -254,9 +328,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$B$1:$I$2</c:f>
+              <c:f>Tabelle1!$B$1:$M$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -265,35 +339,47 @@
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>NEON FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="9">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -302,10 +388,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$I$4</c:f>
+              <c:f>Tabelle1!$B$4:$M$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>5.3</c:v>
                 </c:pt>
@@ -313,21 +399,33 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>599.64</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>237.36</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>237.36</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>23.17</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>9.06</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>9.06</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>107.1</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
+                  <c:v>42.02</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>42.02</c:v>
                 </c:pt>
               </c:numCache>
@@ -350,9 +448,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$B$1:$I$2</c:f>
+              <c:f>Tabelle1!$B$1:$M$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -361,35 +459,47 @@
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>NEON FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="9">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -398,10 +508,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$5:$I$5</c:f>
+              <c:f>Tabelle1!$B$5:$M$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>9.3150999999999993</c:v>
                 </c:pt>
@@ -409,21 +519,33 @@
                   <c:v>2.5546000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2.5546000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>9.3148</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2.5503999999999998</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>2.5503999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>9.3125</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>2.5501999999999998</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>2.5501999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>9.3135999999999992</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
+                  <c:v>2.5514000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>2.5514000000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -432,25 +554,25 @@
         </c:ser>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="52521216"/>
-        <c:axId val="52573696"/>
+        <c:axId val="63711104"/>
+        <c:axId val="63712640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52521216"/>
+        <c:axId val="63711104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52573696"/>
+        <c:crossAx val="63712640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52573696"/>
+        <c:axId val="63712640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4000"/>
@@ -479,7 +601,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52521216"/>
+        <c:crossAx val="63711104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -494,7 +616,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -516,7 +638,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$J$3</c:f>
+              <c:f>Tabelle1!$N$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -527,9 +649,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$K$1:$R$2</c:f>
+              <c:f>Tabelle1!$O$1:$Z$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -538,35 +660,47 @@
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>NEON FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="9">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -575,10 +709,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$K$3:$R$3</c:f>
+              <c:f>Tabelle1!$O$3:$Z$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>99.337368519103805</c:v>
                 </c:pt>
@@ -586,22 +720,34 @@
                   <c:v>99.537702669822366</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>97.543479551615036</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>88.42061163940788</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>89.729469075526183</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>73.310977378835531</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>84.567600631881504</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>84.644664344228687</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>84.227457607777183</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>94.675591114142364</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>94.289900962295064</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70.398495331782797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -612,7 +758,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$J$4</c:f>
+              <c:f>Tabelle1!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -623,9 +769,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$K$1:$R$2</c:f>
+              <c:f>Tabelle1!$O$1:$Z$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -634,35 +780,47 @@
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>NEON FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="9">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -671,10 +829,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$K$4:$R$4</c:f>
+              <c:f>Tabelle1!$O$4:$Z$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.24029577962174814</c:v>
                 </c:pt>
@@ -682,22 +840,34 @@
                   <c:v>0.17102698053234086</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.90879018215790419</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>11.40226571257087</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>10.161348654468938</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>26.405301351502885</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>11.008041048543229</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>11.982510296229872</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>12.308076869781633</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>4.8984327576447564</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>5.3832359217875529</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.907026168316161</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -708,7 +878,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$J$5</c:f>
+              <c:f>Tabelle1!$N$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -719,9 +889,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$K$1:$R$2</c:f>
+              <c:f>Tabelle1!$O$1:$Z$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -730,35 +900,47 @@
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>NEON FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="9">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -767,10 +949,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$K$5:$R$5</c:f>
+              <c:f>Tabelle1!$O$5:$Z$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.42233570127444264</c:v>
                 </c:pt>
@@ -778,22 +960,34 @@
                   <c:v>0.29127034964527865</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.5477302662270547</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.17712264802123798</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.10918227000487689</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>0.28372126966158134</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>4.4243583195752612</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>3.3728253595414373</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>3.4644655224411824</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.42597612821288705</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>0.32686311591739081</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6944784999010434</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -801,29 +995,29 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="54568064"/>
-        <c:axId val="54570368"/>
+        <c:axId val="64424192"/>
+        <c:axId val="64425984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54568064"/>
+        <c:axId val="64424192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54570368"/>
+        <c:crossAx val="64425984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54570368"/>
+        <c:axId val="64425984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
-          <c:min val="80"/>
+          <c:min val="65"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -848,7 +1042,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54568064"/>
+        <c:crossAx val="64424192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -861,7 +1055,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -877,7 +1071,7 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -901,13 +1095,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>104774</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>752474</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -1217,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1228,51 +1422,76 @@
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:26">
       <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
+      <c r="P1" s="6"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3" t="s">
+      <c r="S1" s="6"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3" t="s">
+      <c r="V1" s="6"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:26">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1281,16 +1500,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>0</v>
@@ -1298,7 +1517,9 @@
       <c r="I2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="K2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1306,11 +1527,9 @@
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="N2" s="2"/>
       <c r="O2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1318,13 +1537,37 @@
         <v>1</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="T2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:26">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1335,60 +1578,88 @@
         <v>873</v>
       </c>
       <c r="D3" s="1">
+        <v>161</v>
+      </c>
+      <c r="E3" s="1">
         <v>4650</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>2096</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
+        <v>659</v>
+      </c>
+      <c r="H3" s="1">
         <v>178</v>
       </c>
-      <c r="G3" s="1">
+      <c r="I3" s="1">
         <v>64</v>
       </c>
-      <c r="H3" s="1">
+      <c r="J3" s="1">
+        <v>62</v>
+      </c>
+      <c r="K3" s="1">
         <v>2070</v>
       </c>
-      <c r="I3" s="1">
+      <c r="L3" s="1">
         <v>736</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="M3" s="1">
+        <v>106</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="1">
-        <f>B3/K6*100</f>
+      <c r="O3" s="1">
+        <f>B3/O6*100</f>
         <v>99.337368519103805</v>
       </c>
-      <c r="L3" s="1">
-        <f t="shared" ref="L3:R3" si="0">C3/L6*100</f>
+      <c r="P3" s="1">
+        <f>C3/P6*100</f>
         <v>99.537702669822366</v>
       </c>
-      <c r="M3" s="1">
-        <f t="shared" si="0"/>
+      <c r="Q3" s="1">
+        <f>D3/Q6*100</f>
+        <v>97.543479551615036</v>
+      </c>
+      <c r="R3" s="1">
+        <f>E3/R6*100</f>
         <v>88.42061163940788</v>
       </c>
-      <c r="N3" s="1">
-        <f t="shared" si="0"/>
+      <c r="S3" s="1">
+        <f>F3/S6*100</f>
         <v>89.729469075526183</v>
       </c>
-      <c r="O3" s="1">
-        <f t="shared" si="0"/>
+      <c r="T3" s="1">
+        <f>G3/T6*100</f>
+        <v>73.310977378835531</v>
+      </c>
+      <c r="U3" s="1">
+        <f>H3/U6*100</f>
         <v>84.567600631881504</v>
       </c>
-      <c r="P3" s="1">
-        <f t="shared" si="0"/>
+      <c r="V3" s="1">
+        <f>I3/V6*100</f>
         <v>84.644664344228687</v>
       </c>
-      <c r="Q3" s="1">
-        <f t="shared" si="0"/>
+      <c r="W3" s="1">
+        <f>J3/W6*100</f>
+        <v>84.227457607777183</v>
+      </c>
+      <c r="X3" s="1">
+        <f>K3/X6*100</f>
         <v>94.675591114142364</v>
       </c>
-      <c r="R3" s="1">
-        <f t="shared" si="0"/>
+      <c r="Y3" s="1">
+        <f>L3/Y6*100</f>
         <v>94.289900962295064</v>
       </c>
+      <c r="Z3" s="1">
+        <f>M3/Z6*100</f>
+        <v>70.398495331782797</v>
+      </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:26">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1399,60 +1670,88 @@
         <v>1.5</v>
       </c>
       <c r="D4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="1">
         <v>599.64</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>237.36</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
+        <v>237.36</v>
+      </c>
+      <c r="H4" s="1">
         <v>23.17</v>
       </c>
-      <c r="G4" s="1">
+      <c r="I4" s="1">
         <v>9.06</v>
       </c>
-      <c r="H4" s="1">
+      <c r="J4" s="1">
+        <v>9.06</v>
+      </c>
+      <c r="K4" s="1">
         <v>107.1</v>
       </c>
-      <c r="I4" s="1">
+      <c r="L4" s="1">
         <v>42.02</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="M4" s="1">
+        <v>42.02</v>
+      </c>
+      <c r="N4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="1">
-        <f>B4/K6*100</f>
+      <c r="O4" s="1">
+        <f>B4/O6*100</f>
         <v>0.24029577962174814</v>
       </c>
-      <c r="L4" s="1">
-        <f t="shared" ref="L4:R4" si="1">C4/L6*100</f>
+      <c r="P4" s="1">
+        <f>C4/P6*100</f>
         <v>0.17102698053234086</v>
       </c>
-      <c r="M4" s="1">
-        <f t="shared" si="1"/>
+      <c r="Q4" s="1">
+        <f>D4/Q6*100</f>
+        <v>0.90879018215790419</v>
+      </c>
+      <c r="R4" s="1">
+        <f>E4/R6*100</f>
         <v>11.40226571257087</v>
       </c>
-      <c r="N4" s="1">
-        <f t="shared" si="1"/>
+      <c r="S4" s="1">
+        <f>F4/S6*100</f>
         <v>10.161348654468938</v>
       </c>
-      <c r="O4" s="1">
-        <f t="shared" si="1"/>
+      <c r="T4" s="1">
+        <f>G4/T6*100</f>
+        <v>26.405301351502885</v>
+      </c>
+      <c r="U4" s="1">
+        <f>H4/U6*100</f>
         <v>11.008041048543229</v>
       </c>
-      <c r="P4" s="1">
-        <f t="shared" si="1"/>
+      <c r="V4" s="1">
+        <f>I4/V6*100</f>
         <v>11.982510296229872</v>
       </c>
-      <c r="Q4" s="1">
-        <f t="shared" si="1"/>
+      <c r="W4" s="1">
+        <f>J4/W6*100</f>
+        <v>12.308076869781633</v>
+      </c>
+      <c r="X4" s="1">
+        <f>K4/X6*100</f>
         <v>4.8984327576447564</v>
       </c>
-      <c r="R4" s="1">
-        <f t="shared" si="1"/>
+      <c r="Y4" s="1">
+        <f>L4/Y6*100</f>
         <v>5.3832359217875529</v>
       </c>
+      <c r="Z4" s="1">
+        <f>M4/Z6*100</f>
+        <v>27.907026168316161</v>
+      </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:26">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1463,103 +1762,147 @@
         <v>2.5546000000000002</v>
       </c>
       <c r="D5" s="1">
+        <v>2.5546000000000002</v>
+      </c>
+      <c r="E5" s="1">
         <v>9.3148</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>2.5503999999999998</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
+        <v>2.5503999999999998</v>
+      </c>
+      <c r="H5" s="1">
         <v>9.3125</v>
       </c>
-      <c r="G5" s="1">
+      <c r="I5" s="1">
         <v>2.5501999999999998</v>
       </c>
-      <c r="H5" s="1">
+      <c r="J5" s="1">
+        <v>2.5501999999999998</v>
+      </c>
+      <c r="K5" s="1">
         <v>9.3135999999999992</v>
       </c>
-      <c r="I5" s="1">
+      <c r="L5" s="1">
         <v>2.5514000000000001</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="M5" s="1">
+        <v>2.5514000000000001</v>
+      </c>
+      <c r="N5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="1">
-        <f>B5/K6*100</f>
+      <c r="O5" s="1">
+        <f>B5/O6*100</f>
         <v>0.42233570127444264</v>
       </c>
-      <c r="L5" s="1">
-        <f t="shared" ref="L5:R5" si="2">C5/L6*100</f>
+      <c r="P5" s="1">
+        <f>C5/P6*100</f>
         <v>0.29127034964527865</v>
       </c>
-      <c r="M5" s="1">
-        <f t="shared" si="2"/>
+      <c r="Q5" s="1">
+        <f>D5/Q6*100</f>
+        <v>1.5477302662270547</v>
+      </c>
+      <c r="R5" s="1">
+        <f>E5/R6*100</f>
         <v>0.17712264802123798</v>
       </c>
-      <c r="N5" s="1">
-        <f t="shared" si="2"/>
+      <c r="S5" s="1">
+        <f>F5/S6*100</f>
         <v>0.10918227000487689</v>
       </c>
-      <c r="O5" s="1">
-        <f t="shared" si="2"/>
+      <c r="T5" s="1">
+        <f>G5/T6*100</f>
+        <v>0.28372126966158134</v>
+      </c>
+      <c r="U5" s="1">
+        <f>H5/U6*100</f>
         <v>4.4243583195752612</v>
       </c>
-      <c r="P5" s="1">
-        <f t="shared" si="2"/>
+      <c r="V5" s="1">
+        <f>I5/V6*100</f>
         <v>3.3728253595414373</v>
       </c>
-      <c r="Q5" s="1">
-        <f t="shared" si="2"/>
+      <c r="W5" s="1">
+        <f>J5/W6*100</f>
+        <v>3.4644655224411824</v>
+      </c>
+      <c r="X5" s="1">
+        <f>K5/X6*100</f>
         <v>0.42597612821288705</v>
       </c>
-      <c r="R5" s="1">
-        <f t="shared" si="2"/>
+      <c r="Y5" s="1">
+        <f>L5/Y6*100</f>
         <v>0.32686311591739081</v>
       </c>
+      <c r="Z5" s="1">
+        <f>M5/Z6*100</f>
+        <v>1.6944784999010434</v>
+      </c>
     </row>
-    <row r="6" spans="1:18">
-      <c r="K6">
+    <row r="6" spans="1:26">
+      <c r="O6">
         <f>SUM(B3:B5)</f>
         <v>2205.6151</v>
       </c>
-      <c r="L6">
-        <f t="shared" ref="L6:R6" si="3">SUM(C3:C5)</f>
+      <c r="P6">
+        <f>SUM(C3:C5)</f>
         <v>877.05460000000005</v>
       </c>
-      <c r="M6">
-        <f t="shared" si="3"/>
+      <c r="Q6">
+        <f>SUM(D3:D5)</f>
+        <v>165.05459999999999</v>
+      </c>
+      <c r="R6">
+        <f>SUM(E3:E5)</f>
         <v>5258.9548000000004</v>
       </c>
-      <c r="N6">
-        <f t="shared" si="3"/>
+      <c r="S6">
+        <f>SUM(F3:F5)</f>
         <v>2335.9104000000002</v>
       </c>
-      <c r="O6">
-        <f t="shared" si="3"/>
+      <c r="T6">
+        <f>SUM(G3:G5)</f>
+        <v>898.91039999999998</v>
+      </c>
+      <c r="U6">
+        <f>SUM(H3:H5)</f>
         <v>210.48250000000002</v>
       </c>
-      <c r="P6">
-        <f t="shared" si="3"/>
+      <c r="V6">
+        <f>SUM(I3:I5)</f>
         <v>75.610200000000006</v>
       </c>
-      <c r="Q6">
-        <f t="shared" si="3"/>
+      <c r="W6">
+        <f>SUM(J3:J5)</f>
+        <v>73.610200000000006</v>
+      </c>
+      <c r="X6">
+        <f t="shared" ref="X6:Z6" si="0">SUM(K3:K5)</f>
         <v>2186.4135999999999</v>
       </c>
-      <c r="R6">
-        <f t="shared" si="3"/>
+      <c r="Y6">
+        <f t="shared" si="0"/>
         <v>780.57139999999993</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="0"/>
+        <v>150.57140000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="X1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Messungen für DSP_Extraktion durchgeführt und Ergebnisstabellen aktualisiert
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="11">
   <si>
     <t>Unoptimized</t>
   </si>
@@ -47,6 +47,9 @@
   <si>
     <t>NEON FFT Optimized</t>
   </si>
+  <si>
+    <t>DSP</t>
+  </si>
 </sst>
 </file>
 
@@ -69,7 +72,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -129,20 +132,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -150,6 +160,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -208,9 +231,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$B$1:$M$2</c:f>
+              <c:f>Tabelle1!$B$1:$Q$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="16"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -222,44 +245,56 @@
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>DSP</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>NEON FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>DSP</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="8">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="12">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -268,10 +303,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$3:$M$3</c:f>
+              <c:f>Tabelle1!$B$3:$Q$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>2191</c:v>
                 </c:pt>
@@ -282,31 +317,43 @@
                   <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1.9430000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>4650</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2096</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>659</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
+                  <c:v>4.63</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>178</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
+                  <c:v>2.0830000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>2070</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>736</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.849</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -328,9 +375,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$B$1:$M$2</c:f>
+              <c:f>Tabelle1!$B$1:$Q$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="16"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -342,44 +389,56 @@
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>DSP</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>NEON FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>DSP</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="8">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="12">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -388,10 +447,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$M$4</c:f>
+              <c:f>Tabelle1!$B$4:$Q$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>5.3</c:v>
                 </c:pt>
@@ -402,30 +461,42 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>599.64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>237.36</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>237.36</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>237.36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>237.36</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>23.17</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>9.06</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>9.06</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
+                  <c:v>9.06</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>107.1</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>42.02</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
+                  <c:v>42.02</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>42.02</c:v>
                 </c:pt>
               </c:numCache>
@@ -448,9 +519,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$B$1:$M$2</c:f>
+              <c:f>Tabelle1!$B$1:$Q$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="16"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -462,44 +533,56 @@
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>DSP</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>NEON FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>DSP</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="8">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="12">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -508,10 +591,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$5:$M$5</c:f>
+              <c:f>Tabelle1!$B$5:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>9.3150999999999993</c:v>
                 </c:pt>
@@ -522,30 +605,42 @@
                   <c:v>2.5546000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2.5546000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>9.3148</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.5503999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.5503999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>2.5503999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5503999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>9.3125</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>2.5501999999999998</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>2.5501999999999998</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
+                  <c:v>2.5501999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>9.3135999999999992</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>2.5514000000000001</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
+                  <c:v>2.5514000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>2.5514000000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -554,28 +649,28 @@
         </c:ser>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="63711104"/>
-        <c:axId val="63712640"/>
+        <c:axId val="74056448"/>
+        <c:axId val="74057984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="63711104"/>
+        <c:axId val="74056448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63712640"/>
+        <c:crossAx val="74057984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63712640"/>
+        <c:axId val="74057984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4000"/>
+          <c:max val="5500"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -601,7 +696,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63711104"/>
+        <c:crossAx val="74056448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -616,7 +711,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -638,7 +733,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$N$3</c:f>
+              <c:f>Tabelle1!$R$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -649,9 +744,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$O$1:$Z$2</c:f>
+              <c:f>Tabelle1!$S$1:$AH$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="16"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -663,44 +758,56 @@
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>DSP</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>NEON FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>DSP</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="8">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="12">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -709,10 +816,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$O$3:$Z$3</c:f>
+              <c:f>Tabelle1!$S$3:$AH$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>99.337368519103805</c:v>
                 </c:pt>
@@ -723,31 +830,43 @@
                   <c:v>97.543479551615036</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>32.396291850073361</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>88.42061163940788</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>89.729469075526183</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>73.310977378835531</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
+                  <c:v>1.8933476840636558</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>84.567600631881504</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>84.644664344228687</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>84.227457607777183</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
+                  <c:v>15.211930009055591</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>94.675591114142364</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>94.289900962295064</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>70.398495331782797</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.9831625750747515</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -758,7 +877,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$N$4</c:f>
+              <c:f>Tabelle1!$R$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -769,9 +888,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$O$1:$Z$2</c:f>
+              <c:f>Tabelle1!$S$1:$AH$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="16"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -783,44 +902,56 @@
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>DSP</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>NEON FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>DSP</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="8">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="12">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -829,10 +960,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$O$4:$Z$4</c:f>
+              <c:f>Tabelle1!$S$4:$AH$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.24029577962174814</c:v>
                 </c:pt>
@@ -843,31 +974,43 @@
                   <c:v>0.90879018215790419</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>25.010004001600638</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>11.40226571257087</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>10.161348654468938</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>26.405301351502885</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
+                  <c:v>97.063716261198564</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>11.008041048543229</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>11.982510296229872</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>12.308076869781633</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
+                  <c:v>66.164227499780921</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>4.8984327576447564</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>5.3832359217875529</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>27.907026168316161</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90.520547000887547</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -878,7 +1021,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$N$5</c:f>
+              <c:f>Tabelle1!$R$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -889,9 +1032,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$O$1:$Z$2</c:f>
+              <c:f>Tabelle1!$S$1:$AH$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="16"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -903,44 +1046,56 @@
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>Unoptimized</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Unoptimized</c:v>
+                    <c:v>NEON Autocompiler</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>NEON Autocompiler</c:v>
+                    <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>NEON FFT Optimized</c:v>
+                    <c:v>DSP</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>NEON FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>DSP</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="8">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="12">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -949,10 +1104,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$O$5:$Z$5</c:f>
+              <c:f>Tabelle1!$S$5:$AH$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.42233570127444264</c:v>
                 </c:pt>
@@ -963,31 +1118,43 @@
                   <c:v>1.5477302662270547</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>42.593704148325997</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.17712264802123798</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.10918227000487689</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.28372126966158134</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
+                  <c:v>1.0429360547377855</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>4.4243583195752612</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>3.3728253595414373</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>3.4644655224411824</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
+                  <c:v>18.623842491163494</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0.42597612821288705</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>0.32686311591739081</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>1.6944784999010434</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.4962904240377082</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -995,25 +1162,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="64424192"/>
-        <c:axId val="64425984"/>
+        <c:axId val="45876736"/>
+        <c:axId val="45878272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="64424192"/>
+        <c:axId val="45876736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64425984"/>
+        <c:crossAx val="45878272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64425984"/>
+        <c:axId val="45878272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1042,7 +1209,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64424192"/>
+        <c:crossAx val="45876736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1055,7 +1222,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1071,7 +1238,7 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -1095,13 +1262,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>104774</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>752474</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -1411,10 +1578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:AH6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1423,75 +1590,90 @@
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.5703125" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:34">
       <c r="A1" s="2"/>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="7"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="7"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="4" t="s">
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="6"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="3" t="s">
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:34">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1503,71 +1685,95 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="O2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="P2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="V2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AF2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AG2" s="10" t="s">
         <v>9</v>
       </c>
+      <c r="AH2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:34">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1581,85 +1787,113 @@
         <v>161</v>
       </c>
       <c r="E3" s="1">
+        <v>1.9430000000000001</v>
+      </c>
+      <c r="F3" s="1">
         <v>4650</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>2096</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>659</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
+        <v>4.63</v>
+      </c>
+      <c r="J3" s="1">
         <v>178</v>
       </c>
-      <c r="I3" s="1">
+      <c r="K3" s="1">
         <v>64</v>
       </c>
-      <c r="J3" s="1">
+      <c r="L3" s="1">
         <v>62</v>
       </c>
-      <c r="K3" s="1">
+      <c r="M3" s="1">
+        <v>2.0830000000000002</v>
+      </c>
+      <c r="N3" s="1">
         <v>2070</v>
       </c>
-      <c r="L3" s="1">
+      <c r="O3" s="1">
         <v>736</v>
       </c>
-      <c r="M3" s="1">
+      <c r="P3" s="1">
         <v>106</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="Q3" s="1">
+        <v>1.849</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="1">
-        <f>B3/O6*100</f>
+      <c r="S3" s="1">
+        <f>B3/S6*100</f>
         <v>99.337368519103805</v>
       </c>
-      <c r="P3" s="1">
-        <f>C3/P6*100</f>
+      <c r="T3" s="1">
+        <f>C3/T6*100</f>
         <v>99.537702669822366</v>
       </c>
-      <c r="Q3" s="1">
-        <f>D3/Q6*100</f>
+      <c r="U3" s="1">
+        <f>D3/U6*100</f>
         <v>97.543479551615036</v>
       </c>
-      <c r="R3" s="1">
-        <f>E3/R6*100</f>
+      <c r="V3" s="1">
+        <f>E3/V6*100</f>
+        <v>32.396291850073361</v>
+      </c>
+      <c r="W3" s="1">
+        <f>F3/W6*100</f>
         <v>88.42061163940788</v>
       </c>
-      <c r="S3" s="1">
-        <f>F3/S6*100</f>
+      <c r="X3" s="1">
+        <f>G3/X6*100</f>
         <v>89.729469075526183</v>
       </c>
-      <c r="T3" s="1">
-        <f>G3/T6*100</f>
+      <c r="Y3" s="1">
+        <f>H3/Y6*100</f>
         <v>73.310977378835531</v>
       </c>
-      <c r="U3" s="1">
-        <f>H3/U6*100</f>
+      <c r="Z3" s="1">
+        <f>I3/Z6*100</f>
+        <v>1.8933476840636558</v>
+      </c>
+      <c r="AA3" s="1">
+        <f>J3/AA6*100</f>
         <v>84.567600631881504</v>
       </c>
-      <c r="V3" s="1">
-        <f>I3/V6*100</f>
+      <c r="AB3" s="1">
+        <f>K3/AB6*100</f>
         <v>84.644664344228687</v>
       </c>
-      <c r="W3" s="1">
-        <f>J3/W6*100</f>
+      <c r="AC3" s="1">
+        <f>L3/AC6*100</f>
         <v>84.227457607777183</v>
       </c>
-      <c r="X3" s="1">
-        <f>K3/X6*100</f>
+      <c r="AD3" s="1">
+        <f>M3/AD6*100</f>
+        <v>15.211930009055591</v>
+      </c>
+      <c r="AE3" s="1">
+        <f>N3/AE6*100</f>
         <v>94.675591114142364</v>
       </c>
-      <c r="Y3" s="1">
-        <f>L3/Y6*100</f>
+      <c r="AF3" s="1">
+        <f>O3/AF6*100</f>
         <v>94.289900962295064</v>
       </c>
-      <c r="Z3" s="1">
-        <f>M3/Z6*100</f>
+      <c r="AG3" s="1">
+        <f>P3/AG6*100</f>
         <v>70.398495331782797</v>
       </c>
+      <c r="AH3" s="1">
+        <f>Q3/AH6*100</f>
+        <v>3.9831625750747515</v>
+      </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:34">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1673,85 +1907,113 @@
         <v>1.5</v>
       </c>
       <c r="E4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F4" s="1">
         <v>599.64</v>
-      </c>
-      <c r="F4" s="1">
-        <v>237.36</v>
       </c>
       <c r="G4" s="1">
         <v>237.36</v>
       </c>
       <c r="H4" s="1">
+        <v>237.36</v>
+      </c>
+      <c r="I4" s="1">
+        <v>237.36</v>
+      </c>
+      <c r="J4" s="1">
         <v>23.17</v>
       </c>
-      <c r="I4" s="1">
+      <c r="K4" s="1">
         <v>9.06</v>
       </c>
-      <c r="J4" s="1">
+      <c r="L4" s="1">
         <v>9.06</v>
       </c>
-      <c r="K4" s="1">
+      <c r="M4" s="1">
+        <v>9.06</v>
+      </c>
+      <c r="N4" s="1">
         <v>107.1</v>
       </c>
-      <c r="L4" s="1">
+      <c r="O4" s="1">
         <v>42.02</v>
       </c>
-      <c r="M4" s="1">
+      <c r="P4" s="1">
         <v>42.02</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="Q4" s="1">
+        <v>42.02</v>
+      </c>
+      <c r="R4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="1">
-        <f>B4/O6*100</f>
+      <c r="S4" s="1">
+        <f>B4/S6*100</f>
         <v>0.24029577962174814</v>
       </c>
-      <c r="P4" s="1">
-        <f>C4/P6*100</f>
+      <c r="T4" s="1">
+        <f>C4/T6*100</f>
         <v>0.17102698053234086</v>
       </c>
-      <c r="Q4" s="1">
-        <f>D4/Q6*100</f>
+      <c r="U4" s="1">
+        <f>D4/U6*100</f>
         <v>0.90879018215790419</v>
       </c>
-      <c r="R4" s="1">
-        <f>E4/R6*100</f>
+      <c r="V4" s="1">
+        <f>E4/V6*100</f>
+        <v>25.010004001600638</v>
+      </c>
+      <c r="W4" s="1">
+        <f>F4/W6*100</f>
         <v>11.40226571257087</v>
       </c>
-      <c r="S4" s="1">
-        <f>F4/S6*100</f>
+      <c r="X4" s="1">
+        <f>G4/X6*100</f>
         <v>10.161348654468938</v>
       </c>
-      <c r="T4" s="1">
-        <f>G4/T6*100</f>
+      <c r="Y4" s="1">
+        <f>H4/Y6*100</f>
         <v>26.405301351502885</v>
       </c>
-      <c r="U4" s="1">
-        <f>H4/U6*100</f>
+      <c r="Z4" s="1">
+        <f>I4/Z6*100</f>
+        <v>97.063716261198564</v>
+      </c>
+      <c r="AA4" s="1">
+        <f>J4/AA6*100</f>
         <v>11.008041048543229</v>
       </c>
-      <c r="V4" s="1">
-        <f>I4/V6*100</f>
+      <c r="AB4" s="1">
+        <f>K4/AB6*100</f>
         <v>11.982510296229872</v>
       </c>
-      <c r="W4" s="1">
-        <f>J4/W6*100</f>
+      <c r="AC4" s="1">
+        <f>L4/AC6*100</f>
         <v>12.308076869781633</v>
       </c>
-      <c r="X4" s="1">
-        <f>K4/X6*100</f>
+      <c r="AD4" s="1">
+        <f>M4/AD6*100</f>
+        <v>66.164227499780921</v>
+      </c>
+      <c r="AE4" s="1">
+        <f>N4/AE6*100</f>
         <v>4.8984327576447564</v>
       </c>
-      <c r="Y4" s="1">
-        <f>L4/Y6*100</f>
+      <c r="AF4" s="1">
+        <f>O4/AF6*100</f>
         <v>5.3832359217875529</v>
       </c>
-      <c r="Z4" s="1">
-        <f>M4/Z6*100</f>
+      <c r="AG4" s="1">
+        <f>P4/AG6*100</f>
         <v>27.907026168316161</v>
       </c>
+      <c r="AH4" s="1">
+        <f>Q4/AH6*100</f>
+        <v>90.520547000887547</v>
+      </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:34">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1765,144 +2027,236 @@
         <v>2.5546000000000002</v>
       </c>
       <c r="E5" s="1">
+        <v>2.5546000000000002</v>
+      </c>
+      <c r="F5" s="1">
         <v>9.3148</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2.5503999999999998</v>
       </c>
       <c r="G5" s="1">
         <v>2.5503999999999998</v>
       </c>
       <c r="H5" s="1">
+        <v>2.5503999999999998</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2.5503999999999998</v>
+      </c>
+      <c r="J5" s="1">
         <v>9.3125</v>
       </c>
-      <c r="I5" s="1">
+      <c r="K5" s="1">
         <v>2.5501999999999998</v>
       </c>
-      <c r="J5" s="1">
+      <c r="L5" s="1">
         <v>2.5501999999999998</v>
       </c>
-      <c r="K5" s="1">
+      <c r="M5" s="1">
+        <v>2.5501999999999998</v>
+      </c>
+      <c r="N5" s="1">
         <v>9.3135999999999992</v>
       </c>
-      <c r="L5" s="1">
+      <c r="O5" s="1">
         <v>2.5514000000000001</v>
       </c>
-      <c r="M5" s="1">
+      <c r="P5" s="1">
         <v>2.5514000000000001</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="Q5" s="1">
+        <v>2.5514000000000001</v>
+      </c>
+      <c r="R5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="1">
-        <f>B5/O6*100</f>
+      <c r="S5" s="1">
+        <f>B5/S6*100</f>
         <v>0.42233570127444264</v>
       </c>
-      <c r="P5" s="1">
-        <f>C5/P6*100</f>
+      <c r="T5" s="1">
+        <f>C5/T6*100</f>
         <v>0.29127034964527865</v>
       </c>
-      <c r="Q5" s="1">
-        <f>D5/Q6*100</f>
+      <c r="U5" s="1">
+        <f>D5/U6*100</f>
         <v>1.5477302662270547</v>
       </c>
-      <c r="R5" s="1">
-        <f>E5/R6*100</f>
+      <c r="V5" s="1">
+        <f>E5/V6*100</f>
+        <v>42.593704148325997</v>
+      </c>
+      <c r="W5" s="1">
+        <f>F5/W6*100</f>
         <v>0.17712264802123798</v>
       </c>
-      <c r="S5" s="1">
-        <f>F5/S6*100</f>
+      <c r="X5" s="1">
+        <f>G5/X6*100</f>
         <v>0.10918227000487689</v>
       </c>
-      <c r="T5" s="1">
-        <f>G5/T6*100</f>
+      <c r="Y5" s="1">
+        <f>H5/Y6*100</f>
         <v>0.28372126966158134</v>
       </c>
-      <c r="U5" s="1">
-        <f>H5/U6*100</f>
+      <c r="Z5" s="1">
+        <f>I5/Z6*100</f>
+        <v>1.0429360547377855</v>
+      </c>
+      <c r="AA5" s="1">
+        <f>J5/AA6*100</f>
         <v>4.4243583195752612</v>
       </c>
-      <c r="V5" s="1">
-        <f>I5/V6*100</f>
+      <c r="AB5" s="1">
+        <f>K5/AB6*100</f>
         <v>3.3728253595414373</v>
       </c>
-      <c r="W5" s="1">
-        <f>J5/W6*100</f>
+      <c r="AC5" s="1">
+        <f>L5/AC6*100</f>
         <v>3.4644655224411824</v>
       </c>
-      <c r="X5" s="1">
-        <f>K5/X6*100</f>
+      <c r="AD5" s="1">
+        <f>M5/AD6*100</f>
+        <v>18.623842491163494</v>
+      </c>
+      <c r="AE5" s="1">
+        <f>N5/AE6*100</f>
         <v>0.42597612821288705</v>
       </c>
-      <c r="Y5" s="1">
-        <f>L5/Y6*100</f>
+      <c r="AF5" s="1">
+        <f>O5/AF6*100</f>
         <v>0.32686311591739081</v>
       </c>
-      <c r="Z5" s="1">
-        <f>M5/Z6*100</f>
+      <c r="AG5" s="1">
+        <f>P5/AG6*100</f>
         <v>1.6944784999010434</v>
       </c>
+      <c r="AH5" s="1">
+        <f>Q5/AH6*100</f>
+        <v>5.4962904240377082</v>
+      </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:34">
+      <c r="B6">
+        <f t="shared" ref="B6:O6" si="0">B5+B4+B3</f>
+        <v>2205.6151</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>877.05460000000005</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>165.05459999999999</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>5258.9547999999995</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>2335.9104000000002</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>898.91039999999998</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>210.48250000000002</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>75.610200000000006</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>73.610200000000006</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>2186.4135999999999</v>
+      </c>
       <c r="O6">
+        <f t="shared" si="0"/>
+        <v>780.57140000000004</v>
+      </c>
+      <c r="P6">
+        <f>P5+P4+P3</f>
+        <v>150.57140000000001</v>
+      </c>
+      <c r="S6">
         <f>SUM(B3:B5)</f>
         <v>2205.6151</v>
       </c>
-      <c r="P6">
+      <c r="T6">
         <f>SUM(C3:C5)</f>
         <v>877.05460000000005</v>
       </c>
-      <c r="Q6">
+      <c r="U6">
         <f>SUM(D3:D5)</f>
         <v>165.05459999999999</v>
       </c>
-      <c r="R6">
+      <c r="V6">
         <f>SUM(E3:E5)</f>
+        <v>5.9976000000000003</v>
+      </c>
+      <c r="W6">
+        <f>SUM(F3:F5)</f>
         <v>5258.9548000000004</v>
       </c>
-      <c r="S6">
-        <f>SUM(F3:F5)</f>
+      <c r="X6">
+        <f>SUM(G3:G5)</f>
         <v>2335.9104000000002</v>
       </c>
-      <c r="T6">
-        <f>SUM(G3:G5)</f>
+      <c r="Y6">
+        <f>SUM(H3:H5)</f>
         <v>898.91039999999998</v>
       </c>
-      <c r="U6">
-        <f>SUM(H3:H5)</f>
+      <c r="Z6">
+        <f>SUM(I3:I5)</f>
+        <v>244.54040000000001</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" ref="AA6:AD6" si="1">SUM(J3:J5)</f>
         <v>210.48250000000002</v>
       </c>
-      <c r="V6">
-        <f>SUM(I3:I5)</f>
+      <c r="AB6">
+        <f t="shared" si="1"/>
         <v>75.610200000000006</v>
       </c>
-      <c r="W6">
-        <f>SUM(J3:J5)</f>
+      <c r="AC6">
+        <f t="shared" si="1"/>
         <v>73.610200000000006</v>
       </c>
-      <c r="X6">
-        <f t="shared" ref="X6:Z6" si="0">SUM(K3:K5)</f>
+      <c r="AD6">
+        <f t="shared" si="1"/>
+        <v>13.693200000000001</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" ref="AE6:AG6" si="2">SUM(N3:N5)</f>
         <v>2186.4135999999999</v>
       </c>
-      <c r="Y6">
-        <f t="shared" si="0"/>
+      <c r="AF6">
+        <f t="shared" si="2"/>
         <v>780.57139999999993</v>
       </c>
-      <c r="Z6">
-        <f t="shared" si="0"/>
+      <c r="AG6">
+        <f>SUM(P3:P5)</f>
         <v>150.57140000000001</v>
+      </c>
+      <c r="AH6">
+        <f>SUM(Q3:Q5)</f>
+        <v>46.420400000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="AA1:AD1"/>
+    <mergeCell ref="W1:Z1"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Messwerte für DSP und DSP mit FFT neugemessen, Tabellen aktualisiert und umstrukturiert, Referenz zur Compileroptimierung des DSP hinzugefügt und irgendwas in den Basics geschrieben
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="12">
   <si>
     <t>Unoptimized</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>DSP</t>
+  </si>
+  <si>
+    <t>DSP FFT Optimized</t>
   </si>
 </sst>
 </file>
@@ -149,17 +152,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -169,10 +170,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -187,29 +184,7 @@
   <c:lang val="de-DE"/>
   <c:style val="26"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>Laufzeitmessungen auf dem ARM ohne aktive Optimierung</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -231,9 +206,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$B$1:$Q$2</c:f>
+              <c:f>Tabelle1!$B$1:$U$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -248,53 +223,65 @@
                     <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="4">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>DSP</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="11">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="12">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="13">
                     <c:v>DSP</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="14">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="16">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="17">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="18">
                     <c:v>DSP</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>DSP FFT Optimized</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="10">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="15">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -303,10 +290,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$3:$Q$3</c:f>
+              <c:f>Tabelle1!$B$3:$U$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>2191</c:v>
                 </c:pt>
@@ -317,43 +304,55 @@
                   <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9430000000000001</c:v>
+                  <c:v>729.50400000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>526.43899999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>4650</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2096</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>659</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.63</c:v>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v>1661.479</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1254.261</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>178</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.0830000000000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
+                  <c:v>413.38099999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>413.40100000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>2070</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>736</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>106</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.849</c:v>
+                <c:pt idx="18">
+                  <c:v>692.07799999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>488.13400000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -375,9 +374,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$B$1:$Q$2</c:f>
+              <c:f>Tabelle1!$B$1:$U$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -392,53 +391,65 @@
                     <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="4">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>DSP</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="11">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="12">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="13">
                     <c:v>DSP</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="14">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="16">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="17">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="18">
                     <c:v>DSP</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>DSP FFT Optimized</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="10">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="15">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -447,10 +458,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$Q$4</c:f>
+              <c:f>Tabelle1!$B$4:$U$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>5.3</c:v>
                 </c:pt>
@@ -464,10 +475,10 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>599.64</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>237.36</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>237.36</c:v>
@@ -476,27 +487,39 @@
                   <c:v>237.36</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>237.36</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>237.36</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>23.17</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.06</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.06</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>9.06</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>9.06</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.06</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>107.1</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>42.02</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>42.02</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
+                  <c:v>42.02</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>42.02</c:v>
                 </c:pt>
               </c:numCache>
@@ -519,9 +542,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$B$1:$Q$2</c:f>
+              <c:f>Tabelle1!$B$1:$U$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -536,53 +559,65 @@
                     <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="4">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>DSP</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="11">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="12">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="13">
                     <c:v>DSP</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="14">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="16">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="17">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="18">
                     <c:v>DSP</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>DSP FFT Optimized</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="10">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="15">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -591,10 +626,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$5:$Q$5</c:f>
+              <c:f>Tabelle1!$B$5:$U$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>9.3150999999999993</c:v>
                 </c:pt>
@@ -608,10 +643,10 @@
                   <c:v>2.5546000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>2.5546000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>9.3148</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.5503999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2.5503999999999998</c:v>
@@ -620,27 +655,39 @@
                   <c:v>2.5503999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>2.5503999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5503999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>9.3125</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.5501999999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.5501999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2.5501999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>2.5501999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5501999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.5501999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>9.3135999999999992</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>2.5514000000000001</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>2.5514000000000001</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
+                  <c:v>2.5514000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>2.5514000000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -649,26 +696,27 @@
         </c:ser>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="74056448"/>
-        <c:axId val="74057984"/>
+        <c:axId val="76088448"/>
+        <c:axId val="76089984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74056448"/>
+        <c:axId val="76088448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74057984"/>
+        <c:crossAx val="76089984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74057984"/>
+        <c:axId val="76089984"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
           <c:max val="5500"/>
         </c:scaling>
@@ -696,7 +744,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74056448"/>
+        <c:crossAx val="76088448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -711,7 +759,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -733,7 +781,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$R$3</c:f>
+              <c:f>Tabelle1!$V$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -744,9 +792,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$S$1:$AH$2</c:f>
+              <c:f>Tabelle1!$W$1:$AP$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -761,53 +809,65 @@
                     <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="4">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>DSP</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="11">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="12">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="13">
                     <c:v>DSP</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="14">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="16">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="17">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="18">
                     <c:v>DSP</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>DSP FFT Optimized</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="10">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="15">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -816,10 +876,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$S$3:$AH$3</c:f>
+              <c:f>Tabelle1!$W$3:$AP$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>99.337368519103805</c:v>
                 </c:pt>
@@ -830,43 +890,55 @@
                   <c:v>97.543479551615036</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.396291850073361</c:v>
+                  <c:v>99.447269788671278</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>99.235692947096808</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>88.42061163940788</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>89.729469075526183</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>73.310977378835531</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.8933476840636558</c:v>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v>87.382363654704292</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>83.943582376158446</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>84.567600631881504</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>84.644664344228687</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>84.227457607777183</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>15.211930009055591</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
+                  <c:v>97.272837649344268</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>97.268260224671721</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>94.675591114142364</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>94.289900962295064</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>70.398495331782797</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.9831625750747515</c:v>
+                <c:pt idx="18">
+                  <c:v>93.94944189189593</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>91.633011416816885</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -877,7 +949,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$R$4</c:f>
+              <c:f>Tabelle1!$V$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -888,9 +960,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$S$1:$AH$2</c:f>
+              <c:f>Tabelle1!$W$1:$AP$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -905,53 +977,65 @@
                     <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="4">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>DSP</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="11">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="12">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="13">
                     <c:v>DSP</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="14">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="16">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="17">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="18">
                     <c:v>DSP</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>DSP FFT Optimized</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="10">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="15">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -960,10 +1044,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$S$4:$AH$4</c:f>
+              <c:f>Tabelle1!$W$4:$AP$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.24029577962174814</c:v>
                 </c:pt>
@@ -974,43 +1058,55 @@
                   <c:v>0.90879018215790419</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.010004001600638</c:v>
+                  <c:v>0.20448264119594536</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.28275553182922469</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>11.40226571257087</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>10.161348654468938</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>26.405301351502885</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>97.063716261198564</c:v>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v>12.483502853229329</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.885727701654575</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>11.008041048543229</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>11.982510296229872</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>12.308076869781633</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>66.164227499780921</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
+                  <c:v>2.1318088468655354</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.1317085290928803</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>4.8984327576447564</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>5.3832359217875529</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>27.907026168316161</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>90.520547000887547</c:v>
+                <c:pt idx="18">
+                  <c:v>5.7042060985863845</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.8880371777721807</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1021,7 +1117,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$R$5</c:f>
+              <c:f>Tabelle1!$V$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1032,9 +1128,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle1!$S$1:$AH$2</c:f>
+              <c:f>Tabelle1!$W$1:$AP$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Unoptimized</c:v>
@@ -1049,53 +1145,65 @@
                     <c:v>DSP</c:v>
                   </c:pt>
                   <c:pt idx="4">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>DSP</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="11">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="12">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="13">
                     <c:v>DSP</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="14">
+                    <c:v>DSP FFT Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>Unoptimized</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="16">
                     <c:v>NEON Autocompiler</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="17">
                     <c:v>NEON FFT Optimized</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="18">
                     <c:v>DSP</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>DSP FFT Optimized</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>FeatureSet 1</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>FeatureSet 2</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="10">
                     <c:v>FeatureSet 3</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="15">
                     <c:v>FeatureSet 4</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1104,10 +1212,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$S$5:$AH$5</c:f>
+              <c:f>Tabelle1!$W$5:$AP$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.42233570127444264</c:v>
                 </c:pt>
@@ -1118,43 +1226,55 @@
                   <c:v>1.5477302662270547</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.593704148325997</c:v>
+                  <c:v>0.34824757013277469</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.48155152107395832</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.17712264802123798</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.10918227000487689</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.28372126966158134</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0429360547377855</c:v>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.13413349206638051</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.17068992218697263</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>4.4243583195752612</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>3.3728253595414373</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>3.4644655224411824</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>18.623842491163494</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
+                  <c:v>0.60005948358460126</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.60003124623539328</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>0.42597612821288705</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>0.32686311591739081</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>1.6944784999010434</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.4962904240377082</c:v>
+                <c:pt idx="18">
+                  <c:v>0.34635200951768924</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.47895140541094583</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1162,25 +1282,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="45876736"/>
-        <c:axId val="45878272"/>
+        <c:axId val="55449472"/>
+        <c:axId val="55451008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45876736"/>
+        <c:axId val="55449472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45878272"/>
+        <c:crossAx val="55451008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45878272"/>
+        <c:axId val="55451008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1209,7 +1329,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45876736"/>
+        <c:crossAx val="55449472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1222,7 +1342,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1238,7 +1358,7 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -1262,13 +1382,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>104774</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
+      <xdr:col>38</xdr:col>
       <xdr:colOff>752474</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -1578,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH6"/>
+  <dimension ref="A1:AP6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:Q1"/>
+      <selection activeCell="AK4" sqref="AK4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1590,90 +1710,107 @@
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5703125" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.5703125" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="19" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.5703125" customWidth="1"/>
-    <col min="27" max="27" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.5703125" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:42">
       <c r="A1" s="2"/>
       <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="7"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="6" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="6" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="9" t="s">
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="6" t="s">
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="T1" s="7"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="X1" s="7"/>
       <c r="Y1" s="7"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="6" t="s">
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="9" t="s">
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="7"/>
+      <c r="AJ1" s="7"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:42">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1688,54 +1825,54 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="P2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="R2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="S2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="T2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="2"/>
-      <c r="S2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="U2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="V2" s="2"/>
       <c r="W2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1749,31 +1886,55 @@
         <v>10</v>
       </c>
       <c r="AA2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AE2" s="10" t="s">
+      <c r="AF2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AF2" s="10" t="s">
+      <c r="AH2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AG2" s="10" t="s">
+      <c r="AI2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="AK2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:42">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1787,113 +1948,141 @@
         <v>161</v>
       </c>
       <c r="E3" s="1">
-        <v>1.9430000000000001</v>
+        <v>729.50400000000002</v>
       </c>
       <c r="F3" s="1">
+        <v>526.43899999999996</v>
+      </c>
+      <c r="G3" s="1">
         <v>4650</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>2096</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>659</v>
       </c>
-      <c r="I3" s="1">
-        <v>4.63</v>
-      </c>
       <c r="J3" s="1">
+        <v>1661.479</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1254.261</v>
+      </c>
+      <c r="L3" s="1">
         <v>178</v>
       </c>
-      <c r="K3" s="1">
+      <c r="M3" s="1">
         <v>64</v>
       </c>
-      <c r="L3" s="1">
+      <c r="N3" s="1">
         <v>62</v>
       </c>
-      <c r="M3" s="1">
-        <v>2.0830000000000002</v>
-      </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
+        <v>413.38099999999997</v>
+      </c>
+      <c r="P3" s="1">
+        <v>413.40100000000001</v>
+      </c>
+      <c r="Q3" s="1">
         <v>2070</v>
       </c>
-      <c r="O3" s="1">
+      <c r="R3" s="1">
         <v>736</v>
       </c>
-      <c r="P3" s="1">
+      <c r="S3" s="1">
         <v>106</v>
       </c>
-      <c r="Q3" s="1">
-        <v>1.849</v>
-      </c>
-      <c r="R3" s="5" t="s">
+      <c r="T3" s="1">
+        <v>692.07799999999997</v>
+      </c>
+      <c r="U3" s="4">
+        <v>488.13400000000001</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="1">
-        <f>B3/S6*100</f>
+      <c r="W3" s="1">
+        <f t="shared" ref="W3:AI3" si="0">B3/W6*100</f>
         <v>99.337368519103805</v>
       </c>
-      <c r="T3" s="1">
-        <f>C3/T6*100</f>
+      <c r="X3" s="1">
+        <f t="shared" si="0"/>
         <v>99.537702669822366</v>
       </c>
-      <c r="U3" s="1">
-        <f>D3/U6*100</f>
+      <c r="Y3" s="1">
+        <f t="shared" si="0"/>
         <v>97.543479551615036</v>
       </c>
-      <c r="V3" s="1">
-        <f>E3/V6*100</f>
-        <v>32.396291850073361</v>
-      </c>
-      <c r="W3" s="1">
-        <f>F3/W6*100</f>
+      <c r="Z3" s="1">
+        <f t="shared" si="0"/>
+        <v>99.447269788671278</v>
+      </c>
+      <c r="AA3" s="1">
+        <f t="shared" si="0"/>
+        <v>99.235692947096808</v>
+      </c>
+      <c r="AB3" s="1">
+        <f t="shared" si="0"/>
         <v>88.42061163940788</v>
       </c>
-      <c r="X3" s="1">
-        <f>G3/X6*100</f>
+      <c r="AC3" s="1">
+        <f t="shared" si="0"/>
         <v>89.729469075526183</v>
       </c>
-      <c r="Y3" s="1">
-        <f>H3/Y6*100</f>
+      <c r="AD3" s="1">
+        <f t="shared" si="0"/>
         <v>73.310977378835531</v>
       </c>
-      <c r="Z3" s="1">
-        <f>I3/Z6*100</f>
-        <v>1.8933476840636558</v>
-      </c>
-      <c r="AA3" s="1">
-        <f>J3/AA6*100</f>
+      <c r="AE3" s="1">
+        <f t="shared" si="0"/>
+        <v>87.382363654704292</v>
+      </c>
+      <c r="AF3" s="1">
+        <f t="shared" si="0"/>
+        <v>83.943582376158446</v>
+      </c>
+      <c r="AG3" s="1">
+        <f t="shared" si="0"/>
         <v>84.567600631881504</v>
       </c>
-      <c r="AB3" s="1">
-        <f>K3/AB6*100</f>
+      <c r="AH3" s="1">
+        <f t="shared" si="0"/>
         <v>84.644664344228687</v>
       </c>
-      <c r="AC3" s="1">
-        <f>L3/AC6*100</f>
+      <c r="AI3" s="1">
+        <f t="shared" si="0"/>
         <v>84.227457607777183</v>
       </c>
-      <c r="AD3" s="1">
-        <f>M3/AD6*100</f>
-        <v>15.211930009055591</v>
-      </c>
-      <c r="AE3" s="1">
-        <f>N3/AE6*100</f>
+      <c r="AJ3" s="1">
+        <f>P3/AJ6*100</f>
+        <v>97.272837649344268</v>
+      </c>
+      <c r="AK3" s="1">
+        <f>P3/AK6*100</f>
+        <v>97.268260224671721</v>
+      </c>
+      <c r="AL3" s="1">
+        <f>Q3/AL6*100</f>
         <v>94.675591114142364</v>
       </c>
-      <c r="AF3" s="1">
-        <f>O3/AF6*100</f>
+      <c r="AM3" s="1">
+        <f>R3/AM6*100</f>
         <v>94.289900962295064</v>
       </c>
-      <c r="AG3" s="1">
-        <f>P3/AG6*100</f>
+      <c r="AN3" s="1">
+        <f>S3/AN6*100</f>
         <v>70.398495331782797</v>
       </c>
-      <c r="AH3" s="1">
-        <f>Q3/AH6*100</f>
-        <v>3.9831625750747515</v>
+      <c r="AO3" s="1">
+        <f>T3/AO6*100</f>
+        <v>93.94944189189593</v>
+      </c>
+      <c r="AP3" s="1">
+        <f>U3/AP6*100</f>
+        <v>91.633011416816885</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:42">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1910,10 +2099,10 @@
         <v>1.5</v>
       </c>
       <c r="F4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G4" s="1">
         <v>599.64</v>
-      </c>
-      <c r="G4" s="1">
-        <v>237.36</v>
       </c>
       <c r="H4" s="1">
         <v>237.36</v>
@@ -1922,98 +2111,126 @@
         <v>237.36</v>
       </c>
       <c r="J4" s="1">
+        <v>237.36</v>
+      </c>
+      <c r="K4" s="1">
+        <v>237.36</v>
+      </c>
+      <c r="L4" s="1">
         <v>23.17</v>
-      </c>
-      <c r="K4" s="1">
-        <v>9.06</v>
-      </c>
-      <c r="L4" s="1">
-        <v>9.06</v>
       </c>
       <c r="M4" s="1">
         <v>9.06</v>
       </c>
       <c r="N4" s="1">
+        <v>9.06</v>
+      </c>
+      <c r="O4" s="1">
+        <v>9.06</v>
+      </c>
+      <c r="P4" s="1">
+        <v>9.06</v>
+      </c>
+      <c r="Q4" s="1">
         <v>107.1</v>
       </c>
-      <c r="O4" s="1">
+      <c r="R4" s="1">
         <v>42.02</v>
       </c>
-      <c r="P4" s="1">
+      <c r="S4" s="1">
         <v>42.02</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="T4" s="1">
         <v>42.02</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="U4" s="1">
+        <v>42.02</v>
+      </c>
+      <c r="V4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="S4" s="1">
-        <f>B4/S6*100</f>
+      <c r="W4" s="1">
+        <f t="shared" ref="W4:AJ4" si="1">B4/W6*100</f>
         <v>0.24029577962174814</v>
       </c>
-      <c r="T4" s="1">
-        <f>C4/T6*100</f>
+      <c r="X4" s="1">
+        <f t="shared" si="1"/>
         <v>0.17102698053234086</v>
       </c>
-      <c r="U4" s="1">
-        <f>D4/U6*100</f>
+      <c r="Y4" s="1">
+        <f t="shared" si="1"/>
         <v>0.90879018215790419</v>
       </c>
-      <c r="V4" s="1">
-        <f>E4/V6*100</f>
-        <v>25.010004001600638</v>
-      </c>
-      <c r="W4" s="1">
-        <f>F4/W6*100</f>
+      <c r="Z4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.20448264119594536</v>
+      </c>
+      <c r="AA4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.28275553182922469</v>
+      </c>
+      <c r="AB4" s="1">
+        <f t="shared" si="1"/>
         <v>11.40226571257087</v>
       </c>
-      <c r="X4" s="1">
-        <f>G4/X6*100</f>
+      <c r="AC4" s="1">
+        <f t="shared" si="1"/>
         <v>10.161348654468938</v>
       </c>
-      <c r="Y4" s="1">
-        <f>H4/Y6*100</f>
+      <c r="AD4" s="1">
+        <f t="shared" si="1"/>
         <v>26.405301351502885</v>
       </c>
-      <c r="Z4" s="1">
-        <f>I4/Z6*100</f>
-        <v>97.063716261198564</v>
-      </c>
-      <c r="AA4" s="1">
-        <f>J4/AA6*100</f>
+      <c r="AE4" s="1">
+        <f t="shared" si="1"/>
+        <v>12.483502853229329</v>
+      </c>
+      <c r="AF4" s="1">
+        <f t="shared" si="1"/>
+        <v>15.885727701654575</v>
+      </c>
+      <c r="AG4" s="1">
+        <f t="shared" si="1"/>
         <v>11.008041048543229</v>
       </c>
-      <c r="AB4" s="1">
-        <f>K4/AB6*100</f>
+      <c r="AH4" s="1">
+        <f t="shared" si="1"/>
         <v>11.982510296229872</v>
       </c>
-      <c r="AC4" s="1">
-        <f>L4/AC6*100</f>
+      <c r="AI4" s="1">
+        <f t="shared" si="1"/>
         <v>12.308076869781633</v>
       </c>
-      <c r="AD4" s="1">
-        <f>M4/AD6*100</f>
-        <v>66.164227499780921</v>
-      </c>
-      <c r="AE4" s="1">
-        <f>N4/AE6*100</f>
+      <c r="AJ4" s="1">
+        <f t="shared" si="1"/>
+        <v>2.1318088468655354</v>
+      </c>
+      <c r="AK4" s="1">
+        <f>P4/AK6*100</f>
+        <v>2.1317085290928803</v>
+      </c>
+      <c r="AL4" s="1">
+        <f>Q4/AL6*100</f>
         <v>4.8984327576447564</v>
       </c>
-      <c r="AF4" s="1">
-        <f>O4/AF6*100</f>
+      <c r="AM4" s="1">
+        <f>R4/AM6*100</f>
         <v>5.3832359217875529</v>
       </c>
-      <c r="AG4" s="1">
-        <f>P4/AG6*100</f>
+      <c r="AN4" s="1">
+        <f>S4/AN6*100</f>
         <v>27.907026168316161</v>
       </c>
-      <c r="AH4" s="1">
-        <f>Q4/AH6*100</f>
-        <v>90.520547000887547</v>
+      <c r="AO4" s="1">
+        <f>T4/AO6*100</f>
+        <v>5.7042060985863845</v>
+      </c>
+      <c r="AP4" s="1">
+        <f>U4/AP6*100</f>
+        <v>7.8880371777721807</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:42">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2030,10 +2247,10 @@
         <v>2.5546000000000002</v>
       </c>
       <c r="F5" s="1">
+        <v>2.5546000000000002</v>
+      </c>
+      <c r="G5" s="1">
         <v>9.3148</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2.5503999999999998</v>
       </c>
       <c r="H5" s="1">
         <v>2.5503999999999998</v>
@@ -2042,221 +2259,297 @@
         <v>2.5503999999999998</v>
       </c>
       <c r="J5" s="1">
+        <v>2.5503999999999998</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2.5503999999999998</v>
+      </c>
+      <c r="L5" s="1">
         <v>9.3125</v>
-      </c>
-      <c r="K5" s="1">
-        <v>2.5501999999999998</v>
-      </c>
-      <c r="L5" s="1">
-        <v>2.5501999999999998</v>
       </c>
       <c r="M5" s="1">
         <v>2.5501999999999998</v>
       </c>
       <c r="N5" s="1">
+        <v>2.5501999999999998</v>
+      </c>
+      <c r="O5" s="1">
+        <v>2.5501999999999998</v>
+      </c>
+      <c r="P5" s="1">
+        <v>2.5501999999999998</v>
+      </c>
+      <c r="Q5" s="1">
         <v>9.3135999999999992</v>
       </c>
-      <c r="O5" s="1">
+      <c r="R5" s="1">
         <v>2.5514000000000001</v>
       </c>
-      <c r="P5" s="1">
+      <c r="S5" s="1">
         <v>2.5514000000000001</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="T5" s="1">
         <v>2.5514000000000001</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="U5" s="1">
+        <v>2.5514000000000001</v>
+      </c>
+      <c r="V5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="S5" s="1">
-        <f>B5/S6*100</f>
+      <c r="W5" s="1">
+        <f t="shared" ref="W5:AP5" si="2">B5/W6*100</f>
         <v>0.42233570127444264</v>
       </c>
-      <c r="T5" s="1">
-        <f>C5/T6*100</f>
+      <c r="X5" s="1">
+        <f t="shared" si="2"/>
         <v>0.29127034964527865</v>
       </c>
-      <c r="U5" s="1">
-        <f>D5/U6*100</f>
+      <c r="Y5" s="1">
+        <f t="shared" si="2"/>
         <v>1.5477302662270547</v>
       </c>
-      <c r="V5" s="1">
-        <f>E5/V6*100</f>
-        <v>42.593704148325997</v>
-      </c>
-      <c r="W5" s="1">
-        <f>F5/W6*100</f>
+      <c r="Z5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.34824757013277469</v>
+      </c>
+      <c r="AA5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.48155152107395832</v>
+      </c>
+      <c r="AB5" s="1">
+        <f t="shared" si="2"/>
         <v>0.17712264802123798</v>
       </c>
-      <c r="X5" s="1">
-        <f>G5/X6*100</f>
+      <c r="AC5" s="1">
+        <f t="shared" si="2"/>
         <v>0.10918227000487689</v>
       </c>
-      <c r="Y5" s="1">
-        <f>H5/Y6*100</f>
+      <c r="AD5" s="1">
+        <f t="shared" si="2"/>
         <v>0.28372126966158134</v>
       </c>
-      <c r="Z5" s="1">
-        <f>I5/Z6*100</f>
-        <v>1.0429360547377855</v>
-      </c>
-      <c r="AA5" s="1">
-        <f>J5/AA6*100</f>
+      <c r="AE5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.13413349206638051</v>
+      </c>
+      <c r="AF5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.17068992218697263</v>
+      </c>
+      <c r="AG5" s="1">
+        <f t="shared" si="2"/>
         <v>4.4243583195752612</v>
       </c>
-      <c r="AB5" s="1">
-        <f>K5/AB6*100</f>
+      <c r="AH5" s="1">
+        <f t="shared" si="2"/>
         <v>3.3728253595414373</v>
       </c>
-      <c r="AC5" s="1">
-        <f>L5/AC6*100</f>
+      <c r="AI5" s="1">
+        <f t="shared" si="2"/>
         <v>3.4644655224411824</v>
       </c>
-      <c r="AD5" s="1">
-        <f>M5/AD6*100</f>
-        <v>18.623842491163494</v>
-      </c>
-      <c r="AE5" s="1">
-        <f>N5/AE6*100</f>
+      <c r="AJ5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.60005948358460126</v>
+      </c>
+      <c r="AK5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.60003124623539328</v>
+      </c>
+      <c r="AL5" s="1">
+        <f t="shared" si="2"/>
         <v>0.42597612821288705</v>
       </c>
-      <c r="AF5" s="1">
-        <f>O5/AF6*100</f>
+      <c r="AM5" s="1">
+        <f t="shared" si="2"/>
         <v>0.32686311591739081</v>
       </c>
-      <c r="AG5" s="1">
-        <f>P5/AG6*100</f>
+      <c r="AN5" s="1">
+        <f t="shared" si="2"/>
         <v>1.6944784999010434</v>
       </c>
-      <c r="AH5" s="1">
-        <f>Q5/AH6*100</f>
-        <v>5.4962904240377082</v>
+      <c r="AO5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.34635200951768924</v>
+      </c>
+      <c r="AP5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.47895140541094583</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:42">
       <c r="B6">
-        <f t="shared" ref="B6:O6" si="0">B5+B4+B3</f>
+        <f t="shared" ref="B6:R6" si="3">B5+B4+B3</f>
         <v>2205.6151</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>877.05460000000005</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>165.05459999999999</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>733.55860000000007</v>
+      </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>530.49360000000001</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
         <v>5258.9547999999995</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
+      <c r="H6">
+        <f t="shared" si="3"/>
         <v>2335.9104000000002</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
+      <c r="I6">
+        <f t="shared" si="3"/>
         <v>898.91039999999998</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>1901.3894</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>1494.1713999999999</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
         <v>210.48250000000002</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
+      <c r="M6">
+        <f t="shared" si="3"/>
         <v>75.610200000000006</v>
       </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
+      <c r="N6">
+        <f t="shared" si="3"/>
         <v>73.610200000000006</v>
       </c>
-      <c r="N6">
-        <f t="shared" si="0"/>
-        <v>2186.4135999999999</v>
-      </c>
       <c r="O6">
-        <f t="shared" si="0"/>
-        <v>780.57140000000004</v>
+        <f>O5+O4+P3</f>
+        <v>425.01120000000003</v>
       </c>
       <c r="P6">
         <f>P5+P4+P3</f>
+        <v>425.01120000000003</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="3"/>
+        <v>2186.4135999999999</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="3"/>
+        <v>780.57140000000004</v>
+      </c>
+      <c r="S6">
+        <f>S5+S4+S3</f>
         <v>150.57140000000001</v>
       </c>
-      <c r="S6">
+      <c r="T6">
+        <f t="shared" ref="T6:U6" si="4">T5+T4+T3</f>
+        <v>736.64940000000001</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="4"/>
+        <v>532.70540000000005</v>
+      </c>
+      <c r="W6">
         <f>SUM(B3:B5)</f>
         <v>2205.6151</v>
       </c>
-      <c r="T6">
+      <c r="X6">
         <f>SUM(C3:C5)</f>
         <v>877.05460000000005</v>
       </c>
-      <c r="U6">
+      <c r="Y6">
         <f>SUM(D3:D5)</f>
         <v>165.05459999999999</v>
       </c>
-      <c r="V6">
+      <c r="Z6">
         <f>SUM(E3:E5)</f>
-        <v>5.9976000000000003</v>
-      </c>
-      <c r="W6">
+        <v>733.55860000000007</v>
+      </c>
+      <c r="AA6">
         <f>SUM(F3:F5)</f>
+        <v>530.49360000000001</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" ref="AB6:AF6" si="5">SUM(G3:G5)</f>
         <v>5258.9548000000004</v>
       </c>
-      <c r="X6">
-        <f>SUM(G3:G5)</f>
+      <c r="AC6">
+        <f t="shared" si="5"/>
         <v>2335.9104000000002</v>
       </c>
-      <c r="Y6">
-        <f>SUM(H3:H5)</f>
+      <c r="AD6">
+        <f t="shared" si="5"/>
         <v>898.91039999999998</v>
       </c>
-      <c r="Z6">
-        <f>SUM(I3:I5)</f>
-        <v>244.54040000000001</v>
-      </c>
-      <c r="AA6">
-        <f t="shared" ref="AA6:AD6" si="1">SUM(J3:J5)</f>
+      <c r="AE6">
+        <f t="shared" si="5"/>
+        <v>1901.3894</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" si="5"/>
+        <v>1494.1714000000002</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" ref="AG6:AJ6" si="6">SUM(L3:L5)</f>
         <v>210.48250000000002</v>
       </c>
-      <c r="AB6">
-        <f t="shared" si="1"/>
+      <c r="AH6">
+        <f t="shared" si="6"/>
         <v>75.610200000000006</v>
       </c>
-      <c r="AC6">
-        <f t="shared" si="1"/>
+      <c r="AI6">
+        <f t="shared" si="6"/>
         <v>73.610200000000006</v>
       </c>
-      <c r="AD6">
-        <f t="shared" si="1"/>
-        <v>13.693200000000001</v>
-      </c>
-      <c r="AE6">
-        <f t="shared" ref="AE6:AG6" si="2">SUM(N3:N5)</f>
+      <c r="AJ6">
+        <f t="shared" si="6"/>
+        <v>424.99119999999999</v>
+      </c>
+      <c r="AK6">
+        <f>SUM(P3:P5)</f>
+        <v>425.01120000000003</v>
+      </c>
+      <c r="AL6">
+        <f t="shared" ref="AL6:AM6" si="7">SUM(Q3:Q5)</f>
         <v>2186.4135999999999</v>
       </c>
-      <c r="AF6">
-        <f t="shared" si="2"/>
+      <c r="AM6">
+        <f t="shared" si="7"/>
         <v>780.57139999999993</v>
       </c>
-      <c r="AG6">
-        <f>SUM(P3:P5)</f>
+      <c r="AN6">
+        <f>SUM(S3:S5)</f>
         <v>150.57140000000001</v>
       </c>
-      <c r="AH6">
-        <f>SUM(Q3:Q5)</f>
-        <v>46.420400000000001</v>
+      <c r="AO6">
+        <f>SUM(T3:T5)</f>
+        <v>736.6493999999999</v>
+      </c>
+      <c r="AP6">
+        <f>SUM(U3:U5)</f>
+        <v>532.70539999999994</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="AA1:AD1"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="AL1:AP1"/>
+    <mergeCell ref="AG1:AK1"/>
+    <mergeCell ref="AB1:AF1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="Q1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fehler bei den Messungen der Klassifikation behoben und neu gemessen, Results.xlsx dahingehend korrigiert
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -158,9 +158,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -168,6 +165,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -646,49 +646,49 @@
                   <c:v>2.5546000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.3148</c:v>
+                  <c:v>28.47</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5503999999999998</c:v>
+                  <c:v>7.65</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5503999999999998</c:v>
+                  <c:v>7.65</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.5503999999999998</c:v>
+                  <c:v>7.65</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.5503999999999998</c:v>
+                  <c:v>7.65</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.3125</c:v>
+                  <c:v>21.17</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.5501999999999998</c:v>
+                  <c:v>6.81</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.5501999999999998</c:v>
+                  <c:v>6.81</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.5501999999999998</c:v>
+                  <c:v>6.81</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.5501999999999998</c:v>
+                  <c:v>6.81</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.3135999999999992</c:v>
+                  <c:v>33.53</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.5514000000000001</c:v>
+                  <c:v>9.24</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.5514000000000001</c:v>
+                  <c:v>9.24</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.5514000000000001</c:v>
+                  <c:v>9.24</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.5514000000000001</c:v>
+                  <c:v>9.24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -696,25 +696,25 @@
         </c:ser>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="76088448"/>
-        <c:axId val="76089984"/>
+        <c:axId val="74249344"/>
+        <c:axId val="74250880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76088448"/>
+        <c:axId val="74249344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76089984"/>
+        <c:crossAx val="74250880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76089984"/>
+        <c:axId val="74250880"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -744,7 +744,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76088448"/>
+        <c:crossAx val="74249344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -896,49 +896,49 @@
                   <c:v>99.235692947096808</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>88.42061163940788</c:v>
+                  <c:v>88.099717512518666</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>89.729469075526183</c:v>
+                  <c:v>89.534004553590108</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>73.310977378835531</c:v>
+                  <c:v>72.89742370106525</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>87.382363654704292</c:v>
+                  <c:v>87.148627660584452</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>83.943582376158446</c:v>
+                  <c:v>83.658057816098605</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84.567600631881504</c:v>
+                  <c:v>80.057569488171254</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>84.644664344228687</c:v>
+                  <c:v>80.130211593839988</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>84.227457607777183</c:v>
+                  <c:v>79.61987928598947</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>97.272837649344268</c:v>
+                  <c:v>96.307521706414207</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>97.268260224671721</c:v>
+                  <c:v>96.303034679724462</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>94.675591114142364</c:v>
+                  <c:v>93.638465052948703</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>94.289900962295064</c:v>
+                  <c:v>93.488809287909973</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>70.398495331782797</c:v>
+                  <c:v>67.404298613760645</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>93.94944189189593</c:v>
+                  <c:v>93.104079167215986</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>91.633011416816885</c:v>
+                  <c:v>90.496742640815427</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1064,49 +1064,49 @@
                   <c:v>0.28275553182922469</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.40226571257087</c:v>
+                  <c:v>11.36088486219499</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.161348654468938</c:v>
+                  <c:v>10.139213416431369</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26.405301351502885</c:v>
+                  <c:v>26.256346721828301</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.483502853229329</c:v>
+                  <c:v>12.450111172946711</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.885727701654575</c:v>
+                  <c:v>15.831694203382844</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.008041048543229</c:v>
+                  <c:v>10.420976882252406</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.982510296229872</c:v>
+                  <c:v>11.343433078752973</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.308076869781633</c:v>
+                  <c:v>11.634775908565558</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.1318088468655354</c:v>
+                  <c:v>2.1106532075638733</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1317085290928803</c:v>
+                  <c:v>2.1105548709323481</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.8984327576447564</c:v>
+                  <c:v>4.8447727570873456</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.3832359217875529</c:v>
+                  <c:v>5.3374996824429042</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>27.907026168316161</c:v>
+                  <c:v>26.720081393870021</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.7042060985863845</c:v>
+                  <c:v>5.6528793092778802</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.8880371777721807</c:v>
+                  <c:v>7.7902238437950739</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1232,49 +1232,49 @@
                   <c:v>0.48155152107395832</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17712264802123798</c:v>
+                  <c:v>0.53939762528632396</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.10918227000487689</c:v>
+                  <c:v>0.32678202997851352</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.28372126966158134</c:v>
+                  <c:v>0.84622957710644797</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13413349206638051</c:v>
+                  <c:v>0.40126116646883359</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.17068992218697263</c:v>
+                  <c:v>0.51024798051853193</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.4243583195752612</c:v>
+                  <c:v>9.5214536295763228</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.3728253595414373</c:v>
+                  <c:v>8.5263553274070354</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.4644655224411824</c:v>
+                  <c:v>8.7453448054449705</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.60005948358460126</c:v>
+                  <c:v>1.5864843646258249</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.60003124623539328</c:v>
+                  <c:v>1.5864104493431885</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.42597612821288705</c:v>
+                  <c:v>1.516762189963947</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.32686311591739081</c:v>
+                  <c:v>1.1736910296471306</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6944784999010434</c:v>
+                  <c:v>5.875619992369324</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.34635200951768924</c:v>
+                  <c:v>1.2430415235061305</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.47895140541094583</c:v>
+                  <c:v>1.7130335153894929</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1282,25 +1282,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="55449472"/>
-        <c:axId val="55451008"/>
+        <c:axId val="46732800"/>
+        <c:axId val="46734336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="55449472"/>
+        <c:axId val="46732800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55451008"/>
+        <c:crossAx val="46734336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55451008"/>
+        <c:axId val="46734336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1329,7 +1329,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55449472"/>
+        <c:crossAx val="46732800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1342,7 +1342,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1700,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AK4" sqref="AK4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1752,63 +1752,63 @@
   <sheetData>
     <row r="1" spans="1:42">
       <c r="A1" s="2"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="6" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="6" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="5" t="s">
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
       <c r="V1" s="2"/>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="6" t="s">
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="6" t="s">
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AH1" s="7"/>
-      <c r="AI1" s="7"/>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="5" t="s">
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="7"/>
+      <c r="AL1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
-      <c r="AP1" s="5"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="8"/>
     </row>
     <row r="2" spans="1:42">
       <c r="A2" s="2"/>
@@ -2023,63 +2023,63 @@
       </c>
       <c r="AB3" s="1">
         <f t="shared" si="0"/>
-        <v>88.42061163940788</v>
+        <v>88.099717512518666</v>
       </c>
       <c r="AC3" s="1">
         <f t="shared" si="0"/>
-        <v>89.729469075526183</v>
+        <v>89.534004553590108</v>
       </c>
       <c r="AD3" s="1">
         <f t="shared" si="0"/>
-        <v>73.310977378835531</v>
+        <v>72.89742370106525</v>
       </c>
       <c r="AE3" s="1">
         <f t="shared" si="0"/>
-        <v>87.382363654704292</v>
+        <v>87.148627660584452</v>
       </c>
       <c r="AF3" s="1">
         <f t="shared" si="0"/>
-        <v>83.943582376158446</v>
+        <v>83.658057816098605</v>
       </c>
       <c r="AG3" s="1">
         <f t="shared" si="0"/>
-        <v>84.567600631881504</v>
+        <v>80.057569488171254</v>
       </c>
       <c r="AH3" s="1">
         <f t="shared" si="0"/>
-        <v>84.644664344228687</v>
+        <v>80.130211593839988</v>
       </c>
       <c r="AI3" s="1">
         <f t="shared" si="0"/>
-        <v>84.227457607777183</v>
+        <v>79.61987928598947</v>
       </c>
       <c r="AJ3" s="1">
         <f>P3/AJ6*100</f>
-        <v>97.272837649344268</v>
+        <v>96.307521706414207</v>
       </c>
       <c r="AK3" s="1">
-        <f>P3/AK6*100</f>
-        <v>97.268260224671721</v>
+        <f t="shared" ref="AK3:AP3" si="1">P3/AK6*100</f>
+        <v>96.303034679724462</v>
       </c>
       <c r="AL3" s="1">
-        <f>Q3/AL6*100</f>
-        <v>94.675591114142364</v>
+        <f t="shared" si="1"/>
+        <v>93.638465052948703</v>
       </c>
       <c r="AM3" s="1">
-        <f>R3/AM6*100</f>
-        <v>94.289900962295064</v>
+        <f t="shared" si="1"/>
+        <v>93.488809287909973</v>
       </c>
       <c r="AN3" s="1">
-        <f>S3/AN6*100</f>
-        <v>70.398495331782797</v>
+        <f t="shared" si="1"/>
+        <v>67.404298613760645</v>
       </c>
       <c r="AO3" s="1">
-        <f>T3/AO6*100</f>
-        <v>93.94944189189593</v>
+        <f t="shared" si="1"/>
+        <v>93.104079167215986</v>
       </c>
       <c r="AP3" s="1">
-        <f>U3/AP6*100</f>
-        <v>91.633011416816885</v>
+        <f t="shared" si="1"/>
+        <v>90.496742640815427</v>
       </c>
     </row>
     <row r="4" spans="1:42">
@@ -2150,84 +2150,84 @@
         <v>3</v>
       </c>
       <c r="W4" s="1">
-        <f t="shared" ref="W4:AJ4" si="1">B4/W6*100</f>
+        <f t="shared" ref="W4:AJ4" si="2">B4/W6*100</f>
         <v>0.24029577962174814</v>
       </c>
       <c r="X4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17102698053234086</v>
       </c>
       <c r="Y4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.90879018215790419</v>
       </c>
       <c r="Z4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.20448264119594536</v>
       </c>
       <c r="AA4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.28275553182922469</v>
       </c>
       <c r="AB4" s="1">
-        <f t="shared" si="1"/>
-        <v>11.40226571257087</v>
+        <f t="shared" si="2"/>
+        <v>11.36088486219499</v>
       </c>
       <c r="AC4" s="1">
-        <f t="shared" si="1"/>
-        <v>10.161348654468938</v>
+        <f t="shared" si="2"/>
+        <v>10.139213416431369</v>
       </c>
       <c r="AD4" s="1">
-        <f t="shared" si="1"/>
-        <v>26.405301351502885</v>
+        <f t="shared" si="2"/>
+        <v>26.256346721828301</v>
       </c>
       <c r="AE4" s="1">
-        <f t="shared" si="1"/>
-        <v>12.483502853229329</v>
+        <f t="shared" si="2"/>
+        <v>12.450111172946711</v>
       </c>
       <c r="AF4" s="1">
-        <f t="shared" si="1"/>
-        <v>15.885727701654575</v>
+        <f t="shared" si="2"/>
+        <v>15.831694203382844</v>
       </c>
       <c r="AG4" s="1">
-        <f t="shared" si="1"/>
-        <v>11.008041048543229</v>
+        <f t="shared" si="2"/>
+        <v>10.420976882252406</v>
       </c>
       <c r="AH4" s="1">
-        <f t="shared" si="1"/>
-        <v>11.982510296229872</v>
+        <f t="shared" si="2"/>
+        <v>11.343433078752973</v>
       </c>
       <c r="AI4" s="1">
-        <f t="shared" si="1"/>
-        <v>12.308076869781633</v>
+        <f t="shared" si="2"/>
+        <v>11.634775908565558</v>
       </c>
       <c r="AJ4" s="1">
-        <f t="shared" si="1"/>
-        <v>2.1318088468655354</v>
+        <f t="shared" si="2"/>
+        <v>2.1106532075638733</v>
       </c>
       <c r="AK4" s="1">
-        <f>P4/AK6*100</f>
-        <v>2.1317085290928803</v>
+        <f t="shared" ref="AK4:AP4" si="3">P4/AK6*100</f>
+        <v>2.1105548709323481</v>
       </c>
       <c r="AL4" s="1">
-        <f>Q4/AL6*100</f>
-        <v>4.8984327576447564</v>
+        <f t="shared" si="3"/>
+        <v>4.8447727570873456</v>
       </c>
       <c r="AM4" s="1">
-        <f>R4/AM6*100</f>
-        <v>5.3832359217875529</v>
+        <f t="shared" si="3"/>
+        <v>5.3374996824429042</v>
       </c>
       <c r="AN4" s="1">
-        <f>S4/AN6*100</f>
-        <v>27.907026168316161</v>
+        <f t="shared" si="3"/>
+        <v>26.720081393870021</v>
       </c>
       <c r="AO4" s="1">
-        <f>T4/AO6*100</f>
-        <v>5.7042060985863845</v>
+        <f t="shared" si="3"/>
+        <v>5.6528793092778802</v>
       </c>
       <c r="AP4" s="1">
-        <f>U4/AP6*100</f>
-        <v>7.8880371777721807</v>
+        <f t="shared" si="3"/>
+        <v>7.7902238437950739</v>
       </c>
     </row>
     <row r="5" spans="1:42">
@@ -2250,214 +2250,214 @@
         <v>2.5546000000000002</v>
       </c>
       <c r="G5" s="1">
-        <v>9.3148</v>
+        <v>28.47</v>
       </c>
       <c r="H5" s="1">
-        <v>2.5503999999999998</v>
+        <v>7.65</v>
       </c>
       <c r="I5" s="1">
-        <v>2.5503999999999998</v>
+        <v>7.65</v>
       </c>
       <c r="J5" s="1">
-        <v>2.5503999999999998</v>
+        <v>7.65</v>
       </c>
       <c r="K5" s="1">
-        <v>2.5503999999999998</v>
+        <v>7.65</v>
       </c>
       <c r="L5" s="1">
-        <v>9.3125</v>
+        <v>21.17</v>
       </c>
       <c r="M5" s="1">
-        <v>2.5501999999999998</v>
+        <v>6.81</v>
       </c>
       <c r="N5" s="1">
-        <v>2.5501999999999998</v>
+        <v>6.81</v>
       </c>
       <c r="O5" s="1">
-        <v>2.5501999999999998</v>
+        <v>6.81</v>
       </c>
       <c r="P5" s="1">
-        <v>2.5501999999999998</v>
+        <v>6.81</v>
       </c>
       <c r="Q5" s="1">
-        <v>9.3135999999999992</v>
+        <v>33.53</v>
       </c>
       <c r="R5" s="1">
-        <v>2.5514000000000001</v>
+        <v>9.24</v>
       </c>
       <c r="S5" s="1">
-        <v>2.5514000000000001</v>
+        <v>9.24</v>
       </c>
       <c r="T5" s="1">
-        <v>2.5514000000000001</v>
+        <v>9.24</v>
       </c>
       <c r="U5" s="1">
-        <v>2.5514000000000001</v>
+        <v>9.24</v>
       </c>
       <c r="V5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="W5" s="1">
-        <f t="shared" ref="W5:AP5" si="2">B5/W6*100</f>
+        <f t="shared" ref="W5:AP5" si="4">B5/W6*100</f>
         <v>0.42233570127444264</v>
       </c>
       <c r="X5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.29127034964527865</v>
       </c>
       <c r="Y5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5477302662270547</v>
       </c>
       <c r="Z5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.34824757013277469</v>
       </c>
       <c r="AA5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.48155152107395832</v>
       </c>
       <c r="AB5" s="1">
-        <f t="shared" si="2"/>
-        <v>0.17712264802123798</v>
+        <f t="shared" si="4"/>
+        <v>0.53939762528632396</v>
       </c>
       <c r="AC5" s="1">
-        <f t="shared" si="2"/>
-        <v>0.10918227000487689</v>
+        <f t="shared" si="4"/>
+        <v>0.32678202997851352</v>
       </c>
       <c r="AD5" s="1">
-        <f t="shared" si="2"/>
-        <v>0.28372126966158134</v>
+        <f t="shared" si="4"/>
+        <v>0.84622957710644797</v>
       </c>
       <c r="AE5" s="1">
-        <f t="shared" si="2"/>
-        <v>0.13413349206638051</v>
+        <f t="shared" si="4"/>
+        <v>0.40126116646883359</v>
       </c>
       <c r="AF5" s="1">
-        <f t="shared" si="2"/>
-        <v>0.17068992218697263</v>
+        <f t="shared" si="4"/>
+        <v>0.51024798051853193</v>
       </c>
       <c r="AG5" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4243583195752612</v>
+        <f t="shared" si="4"/>
+        <v>9.5214536295763228</v>
       </c>
       <c r="AH5" s="1">
-        <f t="shared" si="2"/>
-        <v>3.3728253595414373</v>
+        <f t="shared" si="4"/>
+        <v>8.5263553274070354</v>
       </c>
       <c r="AI5" s="1">
-        <f t="shared" si="2"/>
-        <v>3.4644655224411824</v>
+        <f t="shared" si="4"/>
+        <v>8.7453448054449705</v>
       </c>
       <c r="AJ5" s="1">
-        <f t="shared" si="2"/>
-        <v>0.60005948358460126</v>
+        <f t="shared" si="4"/>
+        <v>1.5864843646258249</v>
       </c>
       <c r="AK5" s="1">
-        <f t="shared" si="2"/>
-        <v>0.60003124623539328</v>
+        <f t="shared" si="4"/>
+        <v>1.5864104493431885</v>
       </c>
       <c r="AL5" s="1">
-        <f t="shared" si="2"/>
-        <v>0.42597612821288705</v>
+        <f t="shared" si="4"/>
+        <v>1.516762189963947</v>
       </c>
       <c r="AM5" s="1">
-        <f t="shared" si="2"/>
-        <v>0.32686311591739081</v>
+        <f t="shared" si="4"/>
+        <v>1.1736910296471306</v>
       </c>
       <c r="AN5" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6944784999010434</v>
+        <f t="shared" si="4"/>
+        <v>5.875619992369324</v>
       </c>
       <c r="AO5" s="1">
-        <f t="shared" si="2"/>
-        <v>0.34635200951768924</v>
+        <f t="shared" si="4"/>
+        <v>1.2430415235061305</v>
       </c>
       <c r="AP5" s="1">
-        <f t="shared" si="2"/>
-        <v>0.47895140541094583</v>
+        <f t="shared" si="4"/>
+        <v>1.7130335153894929</v>
       </c>
     </row>
     <row r="6" spans="1:42">
       <c r="B6">
-        <f t="shared" ref="B6:R6" si="3">B5+B4+B3</f>
+        <f t="shared" ref="B6:R6" si="5">B5+B4+B3</f>
         <v>2205.6151</v>
       </c>
       <c r="C6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>877.05460000000005</v>
       </c>
       <c r="D6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>165.05459999999999</v>
       </c>
       <c r="E6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>733.55860000000007</v>
       </c>
       <c r="F6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>530.49360000000001</v>
       </c>
       <c r="G6">
-        <f t="shared" si="3"/>
-        <v>5258.9547999999995</v>
+        <f t="shared" si="5"/>
+        <v>5278.11</v>
       </c>
       <c r="H6">
-        <f t="shared" si="3"/>
-        <v>2335.9104000000002</v>
+        <f>H5+H4+H3</f>
+        <v>2341.0100000000002</v>
       </c>
       <c r="I6">
-        <f t="shared" si="3"/>
-        <v>898.91039999999998</v>
+        <f t="shared" si="5"/>
+        <v>904.01</v>
       </c>
       <c r="J6">
-        <f t="shared" si="3"/>
-        <v>1901.3894</v>
+        <f t="shared" si="5"/>
+        <v>1906.489</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
-        <v>1494.1713999999999</v>
+        <f t="shared" si="5"/>
+        <v>1499.271</v>
       </c>
       <c r="L6">
-        <f t="shared" si="3"/>
-        <v>210.48250000000002</v>
+        <f t="shared" si="5"/>
+        <v>222.34</v>
       </c>
       <c r="M6">
-        <f t="shared" si="3"/>
-        <v>75.610200000000006</v>
+        <f t="shared" si="5"/>
+        <v>79.87</v>
       </c>
       <c r="N6">
-        <f t="shared" si="3"/>
-        <v>73.610200000000006</v>
+        <f t="shared" si="5"/>
+        <v>77.87</v>
       </c>
       <c r="O6">
         <f>O5+O4+P3</f>
-        <v>425.01120000000003</v>
+        <v>429.27100000000002</v>
       </c>
       <c r="P6">
         <f>P5+P4+P3</f>
-        <v>425.01120000000003</v>
+        <v>429.27100000000002</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="3"/>
-        <v>2186.4135999999999</v>
+        <f t="shared" si="5"/>
+        <v>2210.63</v>
       </c>
       <c r="R6">
-        <f t="shared" si="3"/>
-        <v>780.57140000000004</v>
+        <f t="shared" si="5"/>
+        <v>787.26</v>
       </c>
       <c r="S6">
         <f>S5+S4+S3</f>
-        <v>150.57140000000001</v>
+        <v>157.26</v>
       </c>
       <c r="T6">
-        <f t="shared" ref="T6:U6" si="4">T5+T4+T3</f>
-        <v>736.64940000000001</v>
+        <f t="shared" ref="T6:U6" si="6">T5+T4+T3</f>
+        <v>743.33799999999997</v>
       </c>
       <c r="U6">
-        <f t="shared" si="4"/>
-        <v>532.70540000000005</v>
+        <f t="shared" si="6"/>
+        <v>539.39400000000001</v>
       </c>
       <c r="W6">
         <f>SUM(B3:B5)</f>
@@ -2480,64 +2480,64 @@
         <v>530.49360000000001</v>
       </c>
       <c r="AB6">
-        <f t="shared" ref="AB6:AF6" si="5">SUM(G3:G5)</f>
-        <v>5258.9548000000004</v>
+        <f t="shared" ref="AB6:AF6" si="7">SUM(G3:G5)</f>
+        <v>5278.1100000000006</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="5"/>
-        <v>2335.9104000000002</v>
+        <f t="shared" si="7"/>
+        <v>2341.0100000000002</v>
       </c>
       <c r="AD6">
-        <f t="shared" si="5"/>
-        <v>898.91039999999998</v>
+        <f t="shared" si="7"/>
+        <v>904.01</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="5"/>
-        <v>1901.3894</v>
+        <f t="shared" si="7"/>
+        <v>1906.489</v>
       </c>
       <c r="AF6">
-        <f t="shared" si="5"/>
-        <v>1494.1714000000002</v>
+        <f t="shared" si="7"/>
+        <v>1499.2710000000002</v>
       </c>
       <c r="AG6">
-        <f t="shared" ref="AG6:AJ6" si="6">SUM(L3:L5)</f>
-        <v>210.48250000000002</v>
+        <f t="shared" ref="AG6:AJ6" si="8">SUM(L3:L5)</f>
+        <v>222.34000000000003</v>
       </c>
       <c r="AH6">
-        <f t="shared" si="6"/>
-        <v>75.610200000000006</v>
+        <f t="shared" si="8"/>
+        <v>79.87</v>
       </c>
       <c r="AI6">
-        <f t="shared" si="6"/>
-        <v>73.610200000000006</v>
+        <f t="shared" si="8"/>
+        <v>77.87</v>
       </c>
       <c r="AJ6">
-        <f t="shared" si="6"/>
-        <v>424.99119999999999</v>
+        <f t="shared" si="8"/>
+        <v>429.25099999999998</v>
       </c>
       <c r="AK6">
         <f>SUM(P3:P5)</f>
-        <v>425.01120000000003</v>
+        <v>429.27100000000002</v>
       </c>
       <c r="AL6">
-        <f t="shared" ref="AL6:AM6" si="7">SUM(Q3:Q5)</f>
-        <v>2186.4135999999999</v>
+        <f t="shared" ref="AL6:AM6" si="9">SUM(Q3:Q5)</f>
+        <v>2210.63</v>
       </c>
       <c r="AM6">
-        <f t="shared" si="7"/>
-        <v>780.57139999999993</v>
+        <f t="shared" si="9"/>
+        <v>787.26</v>
       </c>
       <c r="AN6">
         <f>SUM(S3:S5)</f>
-        <v>150.57140000000001</v>
+        <v>157.26000000000002</v>
       </c>
       <c r="AO6">
         <f>SUM(T3:T5)</f>
-        <v>736.6493999999999</v>
+        <v>743.33799999999997</v>
       </c>
       <c r="AP6">
         <f>SUM(U3:U5)</f>
-        <v>532.70539999999994</v>
+        <v>539.39400000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ResultsMCL.pdf um fehlende Sets erweitert, MCL Kapitel geschrieben, Rechtschreibprüfung durchgeführt
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="17">
   <si>
     <t>Unoptimized</t>
   </si>
@@ -90,7 +90,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -163,16 +163,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -182,7 +194,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1260,25 +1275,25 @@
         </c:ser>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="58991360"/>
-        <c:axId val="58992896"/>
+        <c:axId val="79520512"/>
+        <c:axId val="79522048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58991360"/>
+        <c:axId val="79520512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58992896"/>
+        <c:crossAx val="79522048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58992896"/>
+        <c:axId val="79522048"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1308,7 +1323,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58991360"/>
+        <c:crossAx val="79520512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2395,25 +2410,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="57099392"/>
-        <c:axId val="57100928"/>
+        <c:axId val="48133248"/>
+        <c:axId val="48134784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57099392"/>
+        <c:axId val="48133248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57100928"/>
+        <c:crossAx val="48134784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57100928"/>
+        <c:axId val="48134784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2442,7 +2457,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57099392"/>
+        <c:crossAx val="48133248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2456,6 +2471,508 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Extraction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Tabelle1!$B$37:$O$38</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="14"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>FeatureSet 1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>FeatureSet 2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>FeatureSet 2d</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>FeatureSet 3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>FeatureSet 3b</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>FeatureSet 4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>FeatureSet 4b</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$39:$O$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>99.353364229161173</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.560928322974291</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.070850631837331</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.527120823171131</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>98.59772129710781</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.146965634901292</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>81.778921253330878</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81.956716609040853</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>98.023018888705323</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>98.416115638935878</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95.566984607713692</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>95.450536909270113</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>99.561831745314095</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>99.66282549526737</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Processing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Tabelle1!$B$37:$O$38</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="14"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>FeatureSet 1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>FeatureSet 2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>FeatureSet 2d</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>FeatureSet 3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>FeatureSet 3b</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>FeatureSet 4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>FeatureSet 4b</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$40:$O$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.23897408922303942</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15966242800935163</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.383488893602836</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.143132338682465</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57612001855957107</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3470631245430173</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.654231370026649</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.640414905877833</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.946379287685636</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1263605549590516</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.4302545682865344</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.7687399491622133</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.15006421016685023</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.11374561605438124</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Classification</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Tabelle1!$B$37:$O$38</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="14"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Unoptimized</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>NEON Autocompiler</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>FeatureSet 1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>FeatureSet 2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>FeatureSet 2d</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>FeatureSet 3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>FeatureSet 3b</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>FeatureSet 4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>FeatureSet 4b</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$41:$O$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.40766168161577315</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27940924901636544</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54566047455983502</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3297468381464127</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82615868433262885</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.50597124055569098</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.5668473766424702</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4028684850813162</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.5711657247995801</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1696152667541539</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0027608239997785</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.7807231415676712</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.28810404451904903</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.22342888867824887</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="75"/>
+        <c:overlap val="100"/>
+        <c:axId val="56791424"/>
+        <c:axId val="56794496"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="56791424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56794496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="56794496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="80"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Anteil in [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56791424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2518,6 +3035,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2811,10 +3358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CV6"/>
+  <dimension ref="A1:CV41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2923,133 +3470,133 @@
   <sheetData>
     <row r="1" spans="1:100">
       <c r="A1" s="2"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="5" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="5" t="s">
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="5" t="s">
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="5" t="s">
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="8" t="s">
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="7"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
-      <c r="AO1" s="8"/>
-      <c r="AP1" s="8"/>
-      <c r="AQ1" s="8"/>
-      <c r="AR1" s="8" t="s">
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AS1" s="8"/>
-      <c r="AT1" s="8"/>
-      <c r="AU1" s="8"/>
-      <c r="AV1" s="8"/>
-      <c r="AW1" s="8"/>
-      <c r="AX1" s="8"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
+      <c r="AW1" s="5"/>
+      <c r="AX1" s="5"/>
       <c r="AY1" s="2"/>
-      <c r="AZ1" s="5" t="s">
+      <c r="AZ1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="BA1" s="6"/>
-      <c r="BB1" s="6"/>
-      <c r="BC1" s="6"/>
-      <c r="BD1" s="6"/>
-      <c r="BE1" s="6"/>
-      <c r="BF1" s="7"/>
-      <c r="BG1" s="5" t="s">
+      <c r="BA1" s="7"/>
+      <c r="BB1" s="7"/>
+      <c r="BC1" s="7"/>
+      <c r="BD1" s="7"/>
+      <c r="BE1" s="7"/>
+      <c r="BF1" s="8"/>
+      <c r="BG1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="BH1" s="6"/>
-      <c r="BI1" s="6"/>
-      <c r="BJ1" s="6"/>
-      <c r="BK1" s="6"/>
-      <c r="BL1" s="6"/>
-      <c r="BM1" s="7"/>
-      <c r="BN1" s="5" t="s">
+      <c r="BH1" s="7"/>
+      <c r="BI1" s="7"/>
+      <c r="BJ1" s="7"/>
+      <c r="BK1" s="7"/>
+      <c r="BL1" s="7"/>
+      <c r="BM1" s="8"/>
+      <c r="BN1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="BO1" s="6"/>
-      <c r="BP1" s="6"/>
-      <c r="BQ1" s="6"/>
-      <c r="BR1" s="6"/>
-      <c r="BS1" s="6"/>
-      <c r="BT1" s="7"/>
-      <c r="BU1" s="5" t="s">
+      <c r="BO1" s="7"/>
+      <c r="BP1" s="7"/>
+      <c r="BQ1" s="7"/>
+      <c r="BR1" s="7"/>
+      <c r="BS1" s="7"/>
+      <c r="BT1" s="8"/>
+      <c r="BU1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="BV1" s="6"/>
-      <c r="BW1" s="6"/>
-      <c r="BX1" s="6"/>
-      <c r="BY1" s="6"/>
-      <c r="BZ1" s="6"/>
-      <c r="CA1" s="7"/>
-      <c r="CB1" s="5" t="s">
+      <c r="BV1" s="7"/>
+      <c r="BW1" s="7"/>
+      <c r="BX1" s="7"/>
+      <c r="BY1" s="7"/>
+      <c r="BZ1" s="7"/>
+      <c r="CA1" s="8"/>
+      <c r="CB1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="CC1" s="6"/>
-      <c r="CD1" s="6"/>
-      <c r="CE1" s="6"/>
-      <c r="CF1" s="6"/>
-      <c r="CG1" s="6"/>
-      <c r="CH1" s="7"/>
-      <c r="CI1" s="8" t="s">
+      <c r="CC1" s="7"/>
+      <c r="CD1" s="7"/>
+      <c r="CE1" s="7"/>
+      <c r="CF1" s="7"/>
+      <c r="CG1" s="7"/>
+      <c r="CH1" s="8"/>
+      <c r="CI1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="CJ1" s="8"/>
-      <c r="CK1" s="8"/>
-      <c r="CL1" s="8"/>
-      <c r="CM1" s="8"/>
-      <c r="CN1" s="8"/>
-      <c r="CO1" s="8"/>
-      <c r="CP1" s="8" t="s">
+      <c r="CJ1" s="5"/>
+      <c r="CK1" s="5"/>
+      <c r="CL1" s="5"/>
+      <c r="CM1" s="5"/>
+      <c r="CN1" s="5"/>
+      <c r="CO1" s="5"/>
+      <c r="CP1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="CQ1" s="8"/>
-      <c r="CR1" s="8"/>
-      <c r="CS1" s="8"/>
-      <c r="CT1" s="8"/>
-      <c r="CU1" s="8"/>
-      <c r="CV1" s="8"/>
+      <c r="CQ1" s="5"/>
+      <c r="CR1" s="5"/>
+      <c r="CS1" s="5"/>
+      <c r="CT1" s="5"/>
+      <c r="CU1" s="5"/>
+      <c r="CV1" s="5"/>
     </row>
     <row r="2" spans="1:100">
       <c r="A2" s="2"/>
@@ -3504,99 +4051,99 @@
         <v>2</v>
       </c>
       <c r="AZ3" s="1">
-        <f>B3/AZ6*100</f>
+        <f t="shared" ref="AZ3:BW3" si="0">B3/AZ6*100</f>
         <v>99.353364229161201</v>
       </c>
       <c r="BA3" s="1">
-        <f>C3/BA6*100</f>
+        <f t="shared" si="0"/>
         <v>99.560928322974291</v>
       </c>
       <c r="BB3" s="1">
-        <f>D3/BB6*100</f>
+        <f t="shared" si="0"/>
         <v>97.664543524416132</v>
       </c>
       <c r="BC3" s="1">
-        <f>E3/BC6*100</f>
+        <f t="shared" si="0"/>
         <v>99.47501479503758</v>
       </c>
       <c r="BD3" s="1">
-        <f>F3/BD6*100</f>
+        <f t="shared" si="0"/>
         <v>98.916237853419062</v>
       </c>
       <c r="BE3" s="1">
-        <f>G3/BE6*100</f>
+        <f t="shared" si="0"/>
         <v>99.273980791606093</v>
       </c>
       <c r="BF3" s="1">
-        <f>H3/BF6*100</f>
+        <f t="shared" si="0"/>
         <v>97.406831147662444</v>
       </c>
       <c r="BG3" s="1">
-        <f>I3/BG6*100</f>
+        <f t="shared" si="0"/>
         <v>88.070850631837331</v>
       </c>
       <c r="BH3" s="1">
-        <f>J3/BH6*100</f>
+        <f t="shared" si="0"/>
         <v>89.527120823171131</v>
       </c>
       <c r="BI3" s="1">
-        <f>K3/BI6*100</f>
+        <f t="shared" si="0"/>
         <v>72.882911777391911</v>
       </c>
       <c r="BJ3" s="1">
-        <f>L3/BJ6*100</f>
+        <f t="shared" si="0"/>
         <v>87.140400352656911</v>
       </c>
       <c r="BK3" s="1">
-        <f>M3/BK6*100</f>
+        <f t="shared" si="0"/>
         <v>76.857427634037961</v>
       </c>
       <c r="BL3" s="1">
-        <f>N3/BL6*100</f>
+        <f t="shared" si="0"/>
         <v>83.648015173553517</v>
       </c>
       <c r="BM3" s="1">
-        <f>O3/BM6*100</f>
+        <f t="shared" si="0"/>
         <v>62.096817826970799</v>
       </c>
       <c r="BN3" s="1">
-        <f>P3/BN6*100</f>
+        <f t="shared" si="0"/>
         <v>98.59772129710781</v>
       </c>
       <c r="BO3" s="1">
-        <f>Q3/BO6*100</f>
+        <f t="shared" si="0"/>
         <v>99.146965634901292</v>
       </c>
       <c r="BP3" s="1">
-        <f>R3/BP6*100</f>
+        <f t="shared" si="0"/>
         <v>97.211155378486055</v>
       </c>
       <c r="BQ3" s="1">
-        <f>S3/BQ6*100</f>
+        <f t="shared" si="0"/>
         <v>98.955276272712283</v>
       </c>
       <c r="BR3" s="1">
-        <f>T3/BR6*100</f>
+        <f t="shared" si="0"/>
         <v>97.888289297126136</v>
       </c>
       <c r="BS3" s="1">
-        <f>U3/BS6*100</f>
+        <f t="shared" si="0"/>
         <v>98.6150614833562</v>
       </c>
       <c r="BT3" s="1">
-        <f>V3/BT6*100</f>
+        <f t="shared" si="0"/>
         <v>95.767057548666742</v>
       </c>
       <c r="BU3" s="1">
-        <f>W3/BU6*100</f>
+        <f t="shared" si="0"/>
         <v>81.778921253330878</v>
       </c>
       <c r="BV3" s="1">
-        <f>X3/BV6*100</f>
+        <f t="shared" si="0"/>
         <v>81.956716609040853</v>
       </c>
       <c r="BW3" s="1">
-        <f>Y3/BW6*100</f>
+        <f t="shared" si="0"/>
         <v>81.482454987514785</v>
       </c>
       <c r="BX3" s="1">
@@ -3636,67 +4183,67 @@
         <v>99.670572762879431</v>
       </c>
       <c r="CG3" s="1">
-        <f>AI3/CG6*100</f>
+        <f t="shared" ref="CG3:CV3" si="1">AI3/CG6*100</f>
         <v>99.751466468483301</v>
       </c>
       <c r="CH3" s="1">
-        <f>AJ3/CH6*100</f>
+        <f t="shared" si="1"/>
         <v>99.671209088674601</v>
       </c>
       <c r="CI3" s="1">
-        <f>AK3/CI6*100</f>
+        <f t="shared" si="1"/>
         <v>95.566984607713692</v>
       </c>
       <c r="CJ3" s="1">
-        <f>AL3/CJ6*100</f>
+        <f t="shared" si="1"/>
         <v>95.450536909270127</v>
       </c>
       <c r="CK3" s="1">
-        <f>AM3/CK6*100</f>
+        <f t="shared" si="1"/>
         <v>75.584632516703778</v>
       </c>
       <c r="CL3" s="1">
-        <f>AN3/CL6*100</f>
+        <f t="shared" si="1"/>
         <v>95.17573897282297</v>
       </c>
       <c r="CM3" s="1">
-        <f>AO3/CM6*100</f>
+        <f t="shared" si="1"/>
         <v>89.874353075650831</v>
       </c>
       <c r="CN3" s="1">
-        <f>AP3/CN6*100</f>
+        <f t="shared" si="1"/>
         <v>93.295286441112054</v>
       </c>
       <c r="CO3" s="1">
-        <f>AQ3/CO6*100</f>
+        <f t="shared" si="1"/>
         <v>74.292644677155778</v>
       </c>
       <c r="CP3" s="1">
-        <f>AR3/CP6*100</f>
+        <f t="shared" si="1"/>
         <v>99.561831745314109</v>
       </c>
       <c r="CQ3" s="1">
-        <f>AS3/CQ6*100</f>
+        <f t="shared" si="1"/>
         <v>99.66282549526737</v>
       </c>
       <c r="CR3" s="1">
-        <f>AT3/CR6*100</f>
+        <f t="shared" si="1"/>
         <v>97.758574129084522</v>
       </c>
       <c r="CS3" s="1">
-        <f>AU3/CS6*100</f>
+        <f t="shared" si="1"/>
         <v>99.641503783646812</v>
       </c>
       <c r="CT3" s="1">
-        <f>AV3/CT6*100</f>
+        <f t="shared" si="1"/>
         <v>99.206645064472056</v>
       </c>
       <c r="CU3" s="1">
-        <f>AW3/CU6*100</f>
+        <f t="shared" si="1"/>
         <v>99.49248304200367</v>
       </c>
       <c r="CV3" s="1">
-        <f>AX3/CV6*100</f>
+        <f t="shared" si="1"/>
         <v>97.602749617306401</v>
       </c>
     </row>
@@ -3855,199 +4402,199 @@
         <v>3</v>
       </c>
       <c r="AZ4" s="1">
-        <f>B4/AZ6*100</f>
+        <f t="shared" ref="AZ4:CE4" si="2">B4/AZ6*100</f>
         <v>0.23897408922303945</v>
       </c>
       <c r="BA4" s="1">
-        <f>C4/BA6*100</f>
+        <f t="shared" si="2"/>
         <v>0.15966242800935163</v>
       </c>
       <c r="BB4" s="1">
-        <f>D4/BB6*100</f>
+        <f t="shared" si="2"/>
         <v>0.84925690021231426</v>
       </c>
       <c r="BC4" s="1">
-        <f>E4/BC6*100</f>
+        <f t="shared" si="2"/>
         <v>0.19090371089542019</v>
       </c>
       <c r="BD4" s="1">
-        <f>F4/BD6*100</f>
+        <f t="shared" si="2"/>
         <v>0.39409532602943326</v>
       </c>
       <c r="BE4" s="1">
-        <f>G4/BE6*100</f>
+        <f t="shared" si="2"/>
         <v>0.26400698487051399</v>
       </c>
       <c r="BF4" s="1">
-        <f>H4/BF6*100</f>
+        <f t="shared" si="2"/>
         <v>0.94297049175911152</v>
       </c>
       <c r="BG4" s="1">
-        <f>I4/BG6*100</f>
+        <f t="shared" si="2"/>
         <v>11.383488893602836</v>
       </c>
       <c r="BH4" s="1">
-        <f>J4/BH6*100</f>
+        <f t="shared" si="2"/>
         <v>10.143132338682467</v>
       </c>
       <c r="BI4" s="1">
-        <f>K4/BI6*100</f>
+        <f t="shared" si="2"/>
         <v>26.263285371437416</v>
       </c>
       <c r="BJ4" s="1">
-        <f>L4/BJ6*100</f>
+        <f t="shared" si="2"/>
         <v>12.454705037948379</v>
       </c>
       <c r="BK4" s="1">
-        <f>M4/BK6*100</f>
+        <f t="shared" si="2"/>
         <v>22.413910272625337</v>
       </c>
       <c r="BL4" s="1">
-        <f>N4/BL6*100</f>
+        <f t="shared" si="2"/>
         <v>15.837129722811882</v>
       </c>
       <c r="BM4" s="1">
-        <f>O4/BM6*100</f>
+        <f t="shared" si="2"/>
         <v>36.70977067021186</v>
       </c>
       <c r="BN4" s="1">
-        <f>P4/BN6*100</f>
+        <f t="shared" si="2"/>
         <v>0.57612001855957107</v>
       </c>
       <c r="BO4" s="1">
-        <f>Q4/BO6*100</f>
+        <f t="shared" si="2"/>
         <v>0.3470631245430173</v>
       </c>
       <c r="BP4" s="1">
-        <f>R4/BP6*100</f>
+        <f t="shared" si="2"/>
         <v>1.1346613545816735</v>
       </c>
       <c r="BQ4" s="1">
-        <f>S4/BQ6*100</f>
+        <f t="shared" si="2"/>
         <v>0.425053310759341</v>
       </c>
       <c r="BR4" s="1">
-        <f>T4/BR6*100</f>
+        <f t="shared" si="2"/>
         <v>0.85916458311210642</v>
       </c>
       <c r="BS4" s="1">
-        <f>U4/BS6*100</f>
+        <f t="shared" si="2"/>
         <v>0.56347212791450418</v>
       </c>
       <c r="BT4" s="1">
-        <f>V4/BT6*100</f>
+        <f t="shared" si="2"/>
         <v>1.722202871628159</v>
       </c>
       <c r="BU4" s="1">
-        <f>W4/BU6*100</f>
+        <f t="shared" si="2"/>
         <v>10.654231370026649</v>
       </c>
       <c r="BV4" s="1">
-        <f>X4/BV6*100</f>
+        <f t="shared" si="2"/>
         <v>11.640414905877833</v>
       </c>
       <c r="BW4" s="1">
-        <f>Y4/BW6*100</f>
+        <f t="shared" si="2"/>
         <v>11.946379287685636</v>
       </c>
       <c r="BX4" s="1">
-        <f>Z4/BX6*100</f>
+        <f t="shared" si="2"/>
         <v>2.1264600405641554</v>
       </c>
       <c r="BY4" s="1">
-        <f>AA4/BY6*100</f>
+        <f t="shared" si="2"/>
         <v>2.785515320334262</v>
       </c>
       <c r="BZ4" s="1">
-        <f>AB4/BZ6*100</f>
+        <f t="shared" si="2"/>
         <v>2.1263605549590516</v>
       </c>
       <c r="CA4" s="1">
-        <f>AC4/CA6*100</f>
+        <f t="shared" si="2"/>
         <v>2.7855323921563824</v>
       </c>
       <c r="CB4" s="1">
-        <f>AD4/CB6*100</f>
+        <f t="shared" si="2"/>
         <v>0.55619802852579991</v>
       </c>
       <c r="CC4" s="1">
-        <f>AE4/CC6*100</f>
+        <f t="shared" si="2"/>
         <v>0.41519298785176073</v>
       </c>
       <c r="CD4" s="1">
-        <f>AF4/CD6*100</f>
+        <f t="shared" si="2"/>
         <v>0.42836744407425037</v>
       </c>
       <c r="CE4" s="1">
-        <f>AG4/CE6*100</f>
+        <f t="shared" si="2"/>
         <v>6.5152710714725254E-2</v>
       </c>
       <c r="CF4" s="1">
-        <f>AH4/CF6*100</f>
+        <f t="shared" ref="CF4:DK4" si="3">AH4/CF6*100</f>
         <v>8.6187358548987958E-2</v>
       </c>
       <c r="CG4" s="1">
-        <f>AI4/CG6*100</f>
+        <f t="shared" si="3"/>
         <v>6.5149566514088E-2</v>
       </c>
       <c r="CH4" s="1">
-        <f>AJ4/CH6*100</f>
+        <f t="shared" si="3"/>
         <v>8.6187908794039647E-2</v>
       </c>
       <c r="CI4" s="1">
-        <f>AK4/CI6*100</f>
+        <f t="shared" si="3"/>
         <v>3.4302545682865344</v>
       </c>
       <c r="CJ4" s="1">
-        <f>AL4/CJ6*100</f>
+        <f t="shared" si="3"/>
         <v>3.7687399491622142</v>
       </c>
       <c r="CK4" s="1">
-        <f>AM4/CK6*100</f>
+        <f t="shared" si="3"/>
         <v>20.225501113585747</v>
       </c>
       <c r="CL4" s="1">
-        <f>AN4/CL6*100</f>
+        <f t="shared" si="3"/>
         <v>3.9963804290126768</v>
       </c>
       <c r="CM4" s="1">
-        <f>AO4/CM6*100</f>
+        <f t="shared" si="3"/>
         <v>8.3880074008434189</v>
       </c>
       <c r="CN4" s="1">
-        <f>AP4/CN6*100</f>
+        <f t="shared" si="3"/>
         <v>5.5541327258062667</v>
       </c>
       <c r="CO4" s="1">
-        <f>AQ4/CO6*100</f>
+        <f t="shared" si="3"/>
         <v>21.295773822173693</v>
       </c>
       <c r="CP4" s="1">
-        <f>AR4/CP6*100</f>
+        <f t="shared" si="3"/>
         <v>0.15006421016685029</v>
       </c>
       <c r="CQ4" s="1">
-        <f>AS4/CQ6*100</f>
+        <f t="shared" si="3"/>
         <v>0.11374561605438124</v>
       </c>
       <c r="CR4" s="1">
-        <f>AT4/CR6*100</f>
+        <f t="shared" si="3"/>
         <v>0.75614366729678628</v>
       </c>
       <c r="CS4" s="1">
-        <f>AU4/CS6*100</f>
+        <f t="shared" si="3"/>
         <v>0.12093848262517133</v>
       </c>
       <c r="CT4" s="1">
-        <f>AV4/CT6*100</f>
+        <f t="shared" si="3"/>
         <v>0.26763780957569849</v>
       </c>
       <c r="CU4" s="1">
-        <f>AW4/CU6*100</f>
+        <f t="shared" si="3"/>
         <v>0.1712105400469606</v>
       </c>
       <c r="CV4" s="1">
-        <f>AX4/CV6*100</f>
+        <f t="shared" si="3"/>
         <v>0.80871097247494428</v>
       </c>
     </row>
@@ -4206,213 +4753,213 @@
         <v>4</v>
       </c>
       <c r="AZ5" s="1">
-        <f>B5/AZ6*100</f>
+        <f t="shared" ref="AZ5:CE5" si="4">B5/AZ6*100</f>
         <v>0.40766168161577326</v>
       </c>
       <c r="BA5" s="1">
-        <f>C5/BA6*100</f>
+        <f t="shared" si="4"/>
         <v>0.27940924901636544</v>
       </c>
       <c r="BB5" s="1">
-        <f>D5/BB6*100</f>
+        <f t="shared" si="4"/>
         <v>1.48619957537155</v>
       </c>
       <c r="BC5" s="1">
-        <f>E5/BC6*100</f>
+        <f t="shared" si="4"/>
         <v>0.3340814940669854</v>
       </c>
       <c r="BD5" s="1">
-        <f>F5/BD6*100</f>
+        <f t="shared" si="4"/>
         <v>0.68966682055150841</v>
       </c>
       <c r="BE5" s="1">
-        <f>G5/BE6*100</f>
+        <f t="shared" si="4"/>
         <v>0.46201222352339955</v>
       </c>
       <c r="BF5" s="1">
-        <f>H5/BF6*100</f>
+        <f t="shared" si="4"/>
         <v>1.6501983605784452</v>
       </c>
       <c r="BG5" s="1">
-        <f>I5/BG6*100</f>
+        <f t="shared" si="4"/>
         <v>0.54566047455983502</v>
       </c>
       <c r="BH5" s="1">
-        <f>J5/BH6*100</f>
+        <f t="shared" si="4"/>
         <v>0.32974683814641276</v>
       </c>
       <c r="BI5" s="1">
-        <f>K5/BI6*100</f>
+        <f t="shared" si="4"/>
         <v>0.8538028511706609</v>
       </c>
       <c r="BJ5" s="1">
-        <f>L5/BJ6*100</f>
+        <f t="shared" si="4"/>
         <v>0.40489460939470873</v>
       </c>
       <c r="BK5" s="1">
-        <f>M5/BK6*100</f>
+        <f t="shared" si="4"/>
         <v>0.72866209333670617</v>
       </c>
       <c r="BL5" s="1">
-        <f>N5/BL6*100</f>
+        <f t="shared" si="4"/>
         <v>0.51485510363459697</v>
       </c>
       <c r="BM5" s="1">
-        <f>O5/BM6*100</f>
+        <f t="shared" si="4"/>
         <v>1.1934115028173478</v>
       </c>
       <c r="BN5" s="1">
-        <f>P5/BN6*100</f>
+        <f t="shared" si="4"/>
         <v>0.82615868433262885</v>
       </c>
       <c r="BO5" s="1">
-        <f>Q5/BO6*100</f>
+        <f t="shared" si="4"/>
         <v>0.50597124055569098</v>
       </c>
       <c r="BP5" s="1">
-        <f>R5/BP6*100</f>
+        <f t="shared" si="4"/>
         <v>1.6541832669322711</v>
       </c>
       <c r="BQ5" s="1">
-        <f>S5/BQ6*100</f>
+        <f t="shared" si="4"/>
         <v>0.61967041652836508</v>
       </c>
       <c r="BR5" s="1">
-        <f>T5/BR6*100</f>
+        <f t="shared" si="4"/>
         <v>1.2525461197617509</v>
       </c>
       <c r="BS5" s="1">
-        <f>U5/BS6*100</f>
+        <f t="shared" si="4"/>
         <v>0.82146638872929134</v>
       </c>
       <c r="BT5" s="1">
-        <f>V5/BT6*100</f>
+        <f t="shared" si="4"/>
         <v>2.5107395797050973</v>
       </c>
       <c r="BU5" s="1">
-        <f>W5/BU6*100</f>
+        <f t="shared" si="4"/>
         <v>7.5668473766424702</v>
       </c>
       <c r="BV5" s="1">
-        <f>X5/BV6*100</f>
+        <f t="shared" si="4"/>
         <v>6.4028684850813162</v>
       </c>
       <c r="BW5" s="1">
-        <f>Y5/BW6*100</f>
+        <f t="shared" si="4"/>
         <v>6.5711657247995801</v>
       </c>
       <c r="BX5" s="1">
-        <f>Z5/BX6*100</f>
+        <f t="shared" si="4"/>
         <v>1.1696699893092164</v>
       </c>
       <c r="BY5" s="1">
-        <f>AA5/BY6*100</f>
+        <f t="shared" si="4"/>
         <v>1.532186644848329</v>
       </c>
       <c r="BZ5" s="1">
-        <f>AB5/BZ6*100</f>
+        <f t="shared" si="4"/>
         <v>1.1696152667541539</v>
       </c>
       <c r="CA5" s="1">
-        <f>AC5/CA6*100</f>
+        <f t="shared" si="4"/>
         <v>1.5321960352895392</v>
       </c>
       <c r="CB5" s="1">
-        <f>AD5/CB6*100</f>
+        <f t="shared" si="4"/>
         <v>1.420783082768875</v>
       </c>
       <c r="CC5" s="1">
-        <f>AE5/CC6*100</f>
+        <f t="shared" si="4"/>
         <v>1.1686913732123634</v>
       </c>
       <c r="CD5" s="1">
-        <f>AF5/CD6*100</f>
+        <f t="shared" si="4"/>
         <v>1.2057750277645565</v>
       </c>
       <c r="CE5" s="1">
-        <f>AG5/CE6*100</f>
+        <f t="shared" si="4"/>
         <v>0.18339281534515253</v>
       </c>
       <c r="CF5" s="1">
-        <f>AH5/CF6*100</f>
+        <f t="shared" ref="CF5:DK5" si="5">AH5/CF6*100</f>
         <v>0.24260145369344757</v>
       </c>
       <c r="CG5" s="1">
-        <f>AI5/CG6*100</f>
+        <f t="shared" si="5"/>
         <v>0.18338396500261805</v>
       </c>
       <c r="CH5" s="1">
-        <f>AJ5/CH6*100</f>
+        <f t="shared" si="5"/>
         <v>0.24260300253137085</v>
       </c>
       <c r="CI5" s="1">
-        <f>AK5/CI6*100</f>
+        <f t="shared" si="5"/>
         <v>1.0027608239997785</v>
       </c>
       <c r="CJ5" s="1">
-        <f>AL5/CJ6*100</f>
+        <f t="shared" si="5"/>
         <v>0.78072314156767131</v>
       </c>
       <c r="CK5" s="1">
-        <f>AM5/CK6*100</f>
+        <f t="shared" si="5"/>
         <v>4.1898663697104679</v>
       </c>
       <c r="CL5" s="1">
-        <f>AN5/CL6*100</f>
+        <f t="shared" si="5"/>
         <v>0.82788059816436055</v>
       </c>
       <c r="CM5" s="1">
-        <f>AO5/CM6*100</f>
+        <f t="shared" si="5"/>
         <v>1.7376395235057598</v>
       </c>
       <c r="CN5" s="1">
-        <f>AP5/CN6*100</f>
+        <f t="shared" si="5"/>
         <v>1.1505808330816836</v>
       </c>
       <c r="CO5" s="1">
-        <f>AQ5/CO6*100</f>
+        <f t="shared" si="5"/>
         <v>4.4115815006705308</v>
       </c>
       <c r="CP5" s="1">
-        <f>AR5/CP6*100</f>
+        <f t="shared" si="5"/>
         <v>0.28810404451904909</v>
       </c>
       <c r="CQ5" s="1">
-        <f>AS5/CQ6*100</f>
+        <f t="shared" si="5"/>
         <v>0.22342888867824887</v>
       </c>
       <c r="CR5" s="1">
-        <f>AT5/CR6*100</f>
+        <f t="shared" si="5"/>
         <v>1.4852822036186875</v>
       </c>
       <c r="CS5" s="1">
-        <f>AU5/CS6*100</f>
+        <f t="shared" si="5"/>
         <v>0.23755773372801511</v>
       </c>
       <c r="CT5" s="1">
-        <f>AV5/CT6*100</f>
+        <f t="shared" si="5"/>
         <v>0.52571712595226483</v>
       </c>
       <c r="CU5" s="1">
-        <f>AW5/CU6*100</f>
+        <f t="shared" si="5"/>
         <v>0.33630641794938693</v>
       </c>
       <c r="CV5" s="1">
-        <f>AX5/CV6*100</f>
+        <f t="shared" si="5"/>
         <v>1.5885394102186405</v>
       </c>
     </row>
     <row r="6" spans="1:100">
       <c r="B6">
-        <f t="shared" ref="B6:AL6" si="0">B5+B4+B3</f>
+        <f t="shared" ref="B6:AL6" si="6">B5+B4+B3</f>
         <v>2205.2600000000002</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>876.85</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>164.85</v>
       </c>
       <c r="E6">
@@ -4424,15 +4971,15 @@
         <v>355.24400000000003</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>530.28899999999999</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>148.46699999999998</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>5279.84</v>
       </c>
       <c r="J6">
@@ -4440,27 +4987,27 @@
         <v>2341.19</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>904.19</v>
       </c>
       <c r="L6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>1906.6690000000001</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6" si="1">M5+M4+M3</f>
+        <f t="shared" ref="M6" si="7">M5+M4+M3</f>
         <v>1059.4759999999999</v>
       </c>
       <c r="N6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>1499.451</v>
       </c>
       <c r="O6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>646.88499999999999</v>
       </c>
       <c r="P6">
-        <f t="shared" ref="P6:V6" si="2">P5+P4+P3</f>
+        <f t="shared" ref="P6" si="8">P5+P4+P3</f>
         <v>2327.64</v>
       </c>
       <c r="Q6">
@@ -4468,35 +5015,35 @@
         <v>1025.75</v>
       </c>
       <c r="R6">
-        <f t="shared" ref="R6:V6" si="3">R5+R4+R3</f>
+        <f t="shared" ref="R6:V6" si="9">R5+R4+R3</f>
         <v>313.75</v>
       </c>
       <c r="S6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>837.54200000000003</v>
       </c>
       <c r="T6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>414.35599999999999</v>
       </c>
       <c r="U6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>631.79700000000003</v>
       </c>
       <c r="V6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>206.71199999999999</v>
       </c>
       <c r="W6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>217.66</v>
       </c>
       <c r="X6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>78.09</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>76.09</v>
       </c>
       <c r="Z6">
@@ -4516,15 +5063,15 @@
         <v>326.32899999999995</v>
       </c>
       <c r="AD6">
-        <f t="shared" ref="AD6:AJ6" si="4">AD5+AD4+AD3</f>
+        <f t="shared" ref="AD6:AF6" si="10">AD5+AD4+AD3</f>
         <v>181.59</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>65.03</v>
       </c>
       <c r="AF6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>63.03</v>
       </c>
       <c r="AG6">
@@ -4544,11 +5091,11 @@
         <v>313.26899999999995</v>
       </c>
       <c r="AK6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>2166.02</v>
       </c>
       <c r="AL6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>771.08</v>
       </c>
       <c r="AM6">
@@ -4556,27 +5103,27 @@
         <v>143.68</v>
       </c>
       <c r="AN6">
-        <f t="shared" ref="AN6:AS6" si="5">AN5+AN4+AN3</f>
+        <f t="shared" ref="AN6:AS6" si="11">AN5+AN4+AN3</f>
         <v>727.15800000000002</v>
       </c>
       <c r="AO6">
-        <f t="shared" ref="AO6" si="6">AO5+AO4+AO3</f>
+        <f t="shared" ref="AO6" si="12">AO5+AO4+AO3</f>
         <v>346.447</v>
       </c>
       <c r="AP6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>523.21400000000006</v>
       </c>
       <c r="AQ6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>136.459</v>
       </c>
       <c r="AR6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>2079.11</v>
       </c>
       <c r="AS6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>738.49</v>
       </c>
       <c r="AT6">
@@ -4584,19 +5131,19 @@
         <v>111.08999999999999</v>
       </c>
       <c r="AU6">
-        <f t="shared" ref="AU6:AX6" si="7">AU5+AU4+AU3</f>
+        <f t="shared" ref="AU6:AX6" si="13">AU5+AU4+AU3</f>
         <v>694.56799999999998</v>
       </c>
       <c r="AV6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>313.85700000000003</v>
       </c>
       <c r="AW6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>490.62400000000002</v>
       </c>
       <c r="AX6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>103.869</v>
       </c>
       <c r="AZ6">
@@ -4620,11 +5167,11 @@
         <v>355.24399999999997</v>
       </c>
       <c r="BE6">
-        <f t="shared" ref="BE6:BF6" si="8">SUM(G3:G5)</f>
+        <f t="shared" ref="BE6:BF6" si="14">SUM(G3:G5)</f>
         <v>530.28899999999999</v>
       </c>
       <c r="BF6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>148.46699999999998</v>
       </c>
       <c r="BG6">
@@ -4648,11 +5195,11 @@
         <v>1059.4759999999999</v>
       </c>
       <c r="BL6">
-        <f t="shared" ref="BL6:BM6" si="9">SUM(N3:N5)</f>
+        <f t="shared" ref="BL6:BM6" si="15">SUM(N3:N5)</f>
         <v>1499.451</v>
       </c>
       <c r="BM6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>646.88499999999999</v>
       </c>
       <c r="BN6">
@@ -4676,31 +5223,31 @@
         <v>414.35599999999999</v>
       </c>
       <c r="BS6">
-        <f t="shared" ref="BS6" si="10">SUM(U3:U5)</f>
+        <f t="shared" ref="BS6" si="16">SUM(U3:U5)</f>
         <v>631.79700000000003</v>
       </c>
       <c r="BT6">
-        <f t="shared" ref="BT6" si="11">SUM(V3:V5)</f>
+        <f t="shared" ref="BT6" si="17">SUM(V3:V5)</f>
         <v>206.71199999999999</v>
       </c>
       <c r="BU6">
-        <f t="shared" ref="BU6:BY6" si="12">SUM(W3:W5)</f>
+        <f t="shared" ref="BU6:BY6" si="18">SUM(W3:W5)</f>
         <v>217.66</v>
       </c>
       <c r="BV6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>78.09</v>
       </c>
       <c r="BW6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>76.09</v>
       </c>
       <c r="BX6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>427.47099999999995</v>
       </c>
       <c r="BY6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>326.33099999999996</v>
       </c>
       <c r="BZ6">
@@ -4712,23 +5259,23 @@
         <v>326.32899999999995</v>
       </c>
       <c r="CB6">
-        <f t="shared" ref="CB6" si="13">SUM(AD3:AD5)</f>
+        <f t="shared" ref="CB6" si="19">SUM(AD3:AD5)</f>
         <v>181.59</v>
       </c>
       <c r="CC6">
-        <f t="shared" ref="CC6" si="14">SUM(AE3:AE5)</f>
+        <f t="shared" ref="CC6" si="20">SUM(AE3:AE5)</f>
         <v>65.03</v>
       </c>
       <c r="CD6">
-        <f t="shared" ref="CD6" si="15">SUM(AF3:AF5)</f>
+        <f t="shared" ref="CD6" si="21">SUM(AF3:AF5)</f>
         <v>63.03</v>
       </c>
       <c r="CE6">
-        <f t="shared" ref="CE6" si="16">SUM(AG3:AG5)</f>
+        <f t="shared" ref="CE6" si="22">SUM(AG3:AG5)</f>
         <v>414.41099999999994</v>
       </c>
       <c r="CF6">
-        <f t="shared" ref="CF6" si="17">SUM(AH3:AH5)</f>
+        <f t="shared" ref="CF6" si="23">SUM(AH3:AH5)</f>
         <v>313.27099999999996</v>
       </c>
       <c r="CG6">
@@ -4740,11 +5287,11 @@
         <v>313.26899999999995</v>
       </c>
       <c r="CI6">
-        <f t="shared" ref="CI6:CJ6" si="18">SUM(AK3:AK5)</f>
+        <f t="shared" ref="CI6:CJ6" si="24">SUM(AK3:AK5)</f>
         <v>2166.02</v>
       </c>
       <c r="CJ6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>771.07999999999993</v>
       </c>
       <c r="CK6">
@@ -4768,11 +5315,11 @@
         <v>136.459</v>
       </c>
       <c r="CP6">
-        <f t="shared" ref="CP6" si="19">SUM(AR3:AR5)</f>
+        <f t="shared" ref="CP6" si="25">SUM(AR3:AR5)</f>
         <v>2079.1099999999997</v>
       </c>
       <c r="CQ6">
-        <f t="shared" ref="CQ6" si="20">SUM(AS3:AS5)</f>
+        <f t="shared" ref="CQ6" si="26">SUM(AS3:AS5)</f>
         <v>738.49</v>
       </c>
       <c r="CR6">
@@ -4796,8 +5343,275 @@
         <v>103.86900000000001</v>
       </c>
     </row>
+    <row r="37" spans="1:17">
+      <c r="B37" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M37" s="10"/>
+      <c r="N37" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O37" s="9"/>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" s="2"/>
+      <c r="B38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="1">
+        <f>B3/B$6*100</f>
+        <v>99.353364229161173</v>
+      </c>
+      <c r="C39" s="1">
+        <f>C3/C$6*100</f>
+        <v>99.560928322974291</v>
+      </c>
+      <c r="D39" s="1">
+        <f>I3/I$6*100</f>
+        <v>88.070850631837331</v>
+      </c>
+      <c r="E39" s="1">
+        <f>J3/J$6*100</f>
+        <v>89.527120823171131</v>
+      </c>
+      <c r="F39" s="1">
+        <f>P3/P$6*100</f>
+        <v>98.59772129710781</v>
+      </c>
+      <c r="G39" s="1">
+        <f>Q3/Q$6*100</f>
+        <v>99.146965634901292</v>
+      </c>
+      <c r="H39" s="1">
+        <f>W3/W$6*100</f>
+        <v>81.778921253330878</v>
+      </c>
+      <c r="I39" s="1">
+        <f>X3/X$6*100</f>
+        <v>81.956716609040853</v>
+      </c>
+      <c r="J39" s="1">
+        <f>AD3/AD$6*100</f>
+        <v>98.023018888705323</v>
+      </c>
+      <c r="K39" s="1">
+        <f t="shared" ref="K39:L39" si="27">AE3/AE$6*100</f>
+        <v>98.416115638935878</v>
+      </c>
+      <c r="L39" s="1">
+        <f>AK3/AK$6*100</f>
+        <v>95.566984607713692</v>
+      </c>
+      <c r="M39" s="1">
+        <f t="shared" ref="M39:N41" si="28">AL3/AL$6*100</f>
+        <v>95.450536909270113</v>
+      </c>
+      <c r="N39" s="1">
+        <f>AR3/AR$6*100</f>
+        <v>99.561831745314095</v>
+      </c>
+      <c r="O39" s="1">
+        <f>AS3/AS$6*100</f>
+        <v>99.66282549526737</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="1">
+        <f t="shared" ref="B40:C41" si="29">B4/B$6*100</f>
+        <v>0.23897408922303942</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="29"/>
+        <v>0.15966242800935163</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" ref="D40:F41" si="30">I4/I$6*100</f>
+        <v>11.383488893602836</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="30"/>
+        <v>10.143132338682465</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" ref="F40:H41" si="31">P4/P$6*100</f>
+        <v>0.57612001855957107</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="31"/>
+        <v>0.3470631245430173</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" ref="H40:J41" si="32">W4/W$6*100</f>
+        <v>10.654231370026649</v>
+      </c>
+      <c r="I40" s="1">
+        <f t="shared" si="32"/>
+        <v>11.640414905877833</v>
+      </c>
+      <c r="J40" s="1">
+        <f t="shared" si="32"/>
+        <v>11.946379287685636</v>
+      </c>
+      <c r="K40" s="1">
+        <f t="shared" ref="K40:K41" si="33">Z4/Z$6*100</f>
+        <v>2.1263605549590516</v>
+      </c>
+      <c r="L40" s="1">
+        <f t="shared" ref="L40:L41" si="34">AK4/AK$6*100</f>
+        <v>3.4302545682865344</v>
+      </c>
+      <c r="M40" s="1">
+        <f t="shared" si="28"/>
+        <v>3.7687399491622133</v>
+      </c>
+      <c r="N40" s="1">
+        <f t="shared" ref="N40:O41" si="35">AR4/AR$6*100</f>
+        <v>0.15006421016685023</v>
+      </c>
+      <c r="O40" s="1">
+        <f t="shared" si="35"/>
+        <v>0.11374561605438124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" si="29"/>
+        <v>0.40766168161577315</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="29"/>
+        <v>0.27940924901636544</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="30"/>
+        <v>0.54566047455983502</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="30"/>
+        <v>0.3297468381464127</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="31"/>
+        <v>0.82615868433262885</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="31"/>
+        <v>0.50597124055569098</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="32"/>
+        <v>7.5668473766424702</v>
+      </c>
+      <c r="I41" s="1">
+        <f t="shared" si="32"/>
+        <v>6.4028684850813162</v>
+      </c>
+      <c r="J41" s="1">
+        <f t="shared" si="32"/>
+        <v>6.5711657247995801</v>
+      </c>
+      <c r="K41" s="1">
+        <f t="shared" si="33"/>
+        <v>1.1696152667541539</v>
+      </c>
+      <c r="L41" s="1">
+        <f t="shared" si="34"/>
+        <v>1.0027608239997785</v>
+      </c>
+      <c r="M41" s="1">
+        <f t="shared" si="28"/>
+        <v>0.7807231415676712</v>
+      </c>
+      <c r="N41" s="1">
+        <f t="shared" si="35"/>
+        <v>0.28810404451904903</v>
+      </c>
+      <c r="O41" s="1">
+        <f t="shared" si="35"/>
+        <v>0.22342888867824887</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="21">
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
     <mergeCell ref="CP1:CV1"/>
     <mergeCell ref="BG1:BM1"/>
     <mergeCell ref="BU1:CA1"/>

</xml_diff>